<commit_message>
fixed GA gradient calculation
</commit_message>
<xml_diff>
--- a/optimizer_outputs_resilience.xlsx
+++ b/optimizer_outputs_resilience.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilyneil/Desktop/rewilding_resilience/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA465F2A-6E32-2D4A-93FD-873C4BF0E0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B8B115-54B2-434E-A930-681129D6CB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="500" windowWidth="21800" windowHeight="16560" xr2:uid="{AE1BBF2D-EC41-B34F-81BF-523AF052BB25}"/>
+    <workbookView xWindow="7000" yWindow="500" windowWidth="21800" windowHeight="16560" activeTab="1" xr2:uid="{AE1BBF2D-EC41-B34F-81BF-523AF052BB25}"/>
   </bookViews>
   <sheets>
     <sheet name="outputs" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="83">
   <si>
     <t>chance_reproduceSapling</t>
   </si>
@@ -172,7 +172,7 @@
     <t>chance_scrub_saves_saplings</t>
   </si>
   <si>
-    <t>run_number</t>
+    <t>fit</t>
   </si>
   <si>
     <t>Done</t>
@@ -677,15 +677,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D6EFC4-B0D4-EA49-B8BA-BDB3C827D59C}">
-  <dimension ref="A1:AW22"/>
+  <dimension ref="A1:AV22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -824,843 +824,291 @@
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
-      <c r="AW1" s="1"/>
-    </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>3.4526878346866001E-3</v>
+        <v>2.07306177012637E-2</v>
       </c>
       <c r="B2" s="1">
-        <v>0.63487402101185697</v>
+        <v>0.36791989849481899</v>
       </c>
       <c r="C2" s="1">
-        <v>0.21860313763992101</v>
+        <v>0.279833453987195</v>
       </c>
       <c r="D2" s="1">
-        <v>3.3937125193391998E-3</v>
+        <v>1.8670200000000001E-3</v>
       </c>
       <c r="E2" s="1">
-        <v>3.4330111481201998E-3</v>
+        <v>3.0390863895783998E-3</v>
       </c>
       <c r="F2" s="1">
-        <v>0.222827431640539</v>
+        <v>0.81766665355022605</v>
       </c>
       <c r="G2" s="1">
-        <v>0.68668703291495503</v>
+        <v>0.83705726999999996</v>
       </c>
       <c r="H2" s="1">
-        <v>0.23251351692311401</v>
+        <v>0.938912040078975</v>
       </c>
       <c r="I2" s="1">
-        <v>2.8954561531048799E-2</v>
+        <v>8.2915355481762196E-2</v>
       </c>
       <c r="J2" s="1">
-        <v>0.150595226088824</v>
+        <v>0.12744690276312801</v>
       </c>
       <c r="K2" s="1">
-        <v>0.30884647216498001</v>
+        <v>0.19678865195313899</v>
       </c>
       <c r="L2" s="1">
-        <v>3.9906904187893E-3</v>
+        <v>1.5923241139799298E-2</v>
       </c>
       <c r="M2" s="1">
-        <v>3.3651990920784601E-2</v>
+        <v>5.4910744572851701E-2</v>
       </c>
       <c r="N2" s="1">
-        <v>9.1426731560706395E-2</v>
+        <v>2.6471378178950001E-2</v>
       </c>
       <c r="O2" s="1">
-        <v>0.55009729119863104</v>
+        <v>0.63389281488985105</v>
       </c>
       <c r="P2" s="1">
-        <v>0.97084189112677</v>
+        <v>2.0989209613724601E-2</v>
       </c>
       <c r="Q2" s="1">
-        <v>0.120899580819619</v>
+        <v>0.17470353760207799</v>
       </c>
       <c r="R2" s="1">
-        <v>0.16882920522755801</v>
+        <v>0.18075157117934901</v>
       </c>
       <c r="S2" s="1">
-        <v>1.50099473478102E-2</v>
+        <v>5.3448301575575001E-3</v>
       </c>
       <c r="T2" s="1">
-        <v>9.1620661165299502E-2</v>
+        <v>8.5698109252469595E-2</v>
       </c>
       <c r="U2" s="1">
-        <v>0.51255313256903301</v>
+        <v>0.41043778180456802</v>
       </c>
       <c r="V2" s="1">
-        <v>0.29014492997698199</v>
+        <v>0.84410096815420399</v>
       </c>
       <c r="W2" s="1">
-        <v>7.2823156486638702E-2</v>
+        <v>0.23421243999999999</v>
       </c>
       <c r="X2" s="1">
-        <v>2.28364713036181E-2</v>
+        <v>0.298063900489144</v>
       </c>
       <c r="Y2" s="1">
-        <v>8.7137950472754005E-3</v>
+        <v>4.67608505202751E-2</v>
       </c>
       <c r="Z2" s="1">
-        <v>4.3972994534562299E-2</v>
+        <v>5.8604597107539597E-2</v>
       </c>
       <c r="AA2" s="1">
-        <v>0.72693454033265903</v>
+        <v>0.42496023035477798</v>
       </c>
       <c r="AB2" s="1">
-        <v>0.20270858100195199</v>
+        <v>5.6174209245325499E-2</v>
       </c>
       <c r="AC2" s="1">
-        <v>0.20233814689583099</v>
+        <v>3.3825955628502102E-2</v>
       </c>
       <c r="AD2" s="1">
-        <v>3.1600016551623297E-2</v>
+        <v>1.2356657523411699E-2</v>
       </c>
       <c r="AE2" s="1">
-        <v>6.1465956204977398E-2</v>
+        <v>3.7052656274977898E-2</v>
       </c>
       <c r="AF2" s="1">
-        <v>0.259582422892288</v>
+        <v>0.115646764697444</v>
       </c>
       <c r="AG2" s="1">
-        <v>0.44486881734002498</v>
+        <v>5.3884223593677498E-2</v>
       </c>
       <c r="AH2" s="1">
-        <v>6.5757563076245E-3</v>
+        <v>1.1418786832505299E-2</v>
       </c>
       <c r="AI2" s="1">
-        <v>0.169138909519749</v>
+        <v>0.21766613578879801</v>
       </c>
       <c r="AJ2" s="1">
-        <v>4.2244305934811301E-2</v>
+        <v>1.11678579741689E-2</v>
       </c>
       <c r="AK2" s="1">
-        <v>7.2780217005104397E-2</v>
+        <v>5.7276742831977499E-2</v>
       </c>
       <c r="AL2" s="1">
-        <v>0.19198668795559201</v>
+        <v>0.34933321383960902</v>
       </c>
       <c r="AM2" s="1">
-        <v>0.63217241092265097</v>
+        <v>0.13987820281646199</v>
       </c>
       <c r="AN2" s="1">
-        <v>0.21223694297055001</v>
+        <v>0.25280292919952702</v>
       </c>
       <c r="AO2" s="1">
-        <v>0.25302744944310002</v>
+        <v>0.32181015720016198</v>
       </c>
       <c r="AP2" s="1">
-        <v>5.7323927578043797E-2</v>
+        <v>6.9184246677001696E-2</v>
       </c>
       <c r="AQ2" s="1">
-        <v>9.2471551226675899E-2</v>
+        <v>3.8138699248282497E-2</v>
       </c>
       <c r="AR2" s="1">
-        <v>0.75948171815090304</v>
-      </c>
-      <c r="AS2" s="1">
-        <v>3</v>
-      </c>
+        <v>0.33475583517440999</v>
+      </c>
+      <c r="AS2" s="1"/>
       <c r="AT2" s="1"/>
       <c r="AU2" s="1"/>
       <c r="AV2" s="1"/>
-      <c r="AW2" s="1"/>
-    </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>2.07306177012637E-2</v>
+        <v>9.4007123711453994E-3</v>
       </c>
       <c r="B3" s="1">
-        <v>0.36791989849481899</v>
+        <v>0.46281241145402002</v>
       </c>
       <c r="C3" s="1">
-        <v>0.279833453987195</v>
+        <v>0.97708446480051203</v>
       </c>
       <c r="D3" s="1">
-        <v>1.8670164546399999E-3</v>
+        <v>5.9498199999999998E-3</v>
       </c>
       <c r="E3" s="1">
-        <v>3.0390863895783998E-3</v>
+        <v>9.9136523316660004E-3</v>
       </c>
       <c r="F3" s="1">
-        <v>0.81766665355022605</v>
+        <v>0.72280092773307802</v>
       </c>
       <c r="G3" s="1">
-        <v>0.83705726579801099</v>
+        <v>0.61098867999999995</v>
       </c>
       <c r="H3" s="1">
-        <v>0.938912040078975</v>
+        <v>0.189896295070247</v>
       </c>
       <c r="I3" s="1">
-        <v>8.2915355481762196E-2</v>
+        <v>2.7248821405216499E-2</v>
       </c>
       <c r="J3" s="1">
-        <v>0.12744690276312801</v>
+        <v>0.10443477827242199</v>
       </c>
       <c r="K3" s="1">
-        <v>0.19678865195313899</v>
+        <v>2.1718387784674002E-2</v>
       </c>
       <c r="L3" s="1">
-        <v>1.5923241139799298E-2</v>
+        <v>3.2579912169592999E-3</v>
       </c>
       <c r="M3" s="1">
-        <v>5.4910744572851701E-2</v>
+        <v>2.8500815512723501E-2</v>
       </c>
       <c r="N3" s="1">
-        <v>2.6471378178950001E-2</v>
+        <v>3.0458041765055899E-2</v>
       </c>
       <c r="O3" s="1">
-        <v>0.63389281488985105</v>
+        <v>0.44252004474949402</v>
       </c>
       <c r="P3" s="1">
-        <v>2.0989209613724601E-2</v>
+        <v>0.70921771659038502</v>
       </c>
       <c r="Q3" s="1">
-        <v>0.17470353760207799</v>
+        <v>0.32178463746241998</v>
       </c>
       <c r="R3" s="1">
-        <v>0.18075157117934901</v>
+        <v>7.8549897149350803E-2</v>
       </c>
       <c r="S3" s="1">
-        <v>5.3448301575575001E-3</v>
+        <v>1.82360276804681E-2</v>
       </c>
       <c r="T3" s="1">
-        <v>8.5698109252469595E-2</v>
+        <v>9.3900620197711008E-3</v>
       </c>
       <c r="U3" s="1">
-        <v>0.41043778180456802</v>
+        <v>0.731290194609307</v>
       </c>
       <c r="V3" s="1">
-        <v>0.84410096815420399</v>
+        <v>0.46669538464035898</v>
       </c>
       <c r="W3" s="1">
-        <v>0.23421244207015501</v>
+        <v>0.20709765999999999</v>
       </c>
       <c r="X3" s="1">
-        <v>0.298063900489144</v>
+        <v>7.6039620229049296E-2</v>
       </c>
       <c r="Y3" s="1">
-        <v>4.67608505202751E-2</v>
+        <v>7.2353529170675404E-2</v>
       </c>
       <c r="Z3" s="1">
-        <v>5.8604597107539597E-2</v>
+        <v>4.1980710199390897E-2</v>
       </c>
       <c r="AA3" s="1">
-        <v>0.42496023035477798</v>
+        <v>0.77126681168856404</v>
       </c>
       <c r="AB3" s="1">
-        <v>5.6174209245325499E-2</v>
+        <v>0.110805698091791</v>
       </c>
       <c r="AC3" s="1">
-        <v>3.3825955628502102E-2</v>
+        <v>3.81399365882392E-2</v>
       </c>
       <c r="AD3" s="1">
-        <v>1.2356657523411699E-2</v>
+        <v>8.0036166686743307E-2</v>
       </c>
       <c r="AE3" s="1">
-        <v>3.7052656274977898E-2</v>
+        <v>2.7184729575304101E-2</v>
       </c>
       <c r="AF3" s="1">
-        <v>0.115646764697444</v>
+        <v>0.338475915628696</v>
       </c>
       <c r="AG3" s="1">
-        <v>5.3884223593677498E-2</v>
+        <v>0.78227418302001295</v>
       </c>
       <c r="AH3" s="1">
-        <v>1.1418786832505299E-2</v>
+        <v>0.118696637821815</v>
       </c>
       <c r="AI3" s="1">
-        <v>0.21766613578879801</v>
+        <v>0.15919674569310299</v>
       </c>
       <c r="AJ3" s="1">
-        <v>1.11678579741689E-2</v>
+        <v>3.6664634935266401E-2</v>
       </c>
       <c r="AK3" s="1">
-        <v>5.7276742831977499E-2</v>
+        <v>8.7221565121345199E-2</v>
       </c>
       <c r="AL3" s="1">
-        <v>0.34933321383960902</v>
+        <v>0.18369111088983001</v>
       </c>
       <c r="AM3" s="1">
-        <v>0.13987820281646199</v>
+        <v>0.992363144426335</v>
       </c>
       <c r="AN3" s="1">
-        <v>0.25280292919952702</v>
+        <v>0.28925486566592901</v>
       </c>
       <c r="AO3" s="1">
-        <v>0.32181015720016198</v>
+        <v>0.26215336739706802</v>
       </c>
       <c r="AP3" s="1">
-        <v>6.9184246677001696E-2</v>
+        <v>5.04783859417232E-2</v>
       </c>
       <c r="AQ3" s="1">
-        <v>3.8138699248282497E-2</v>
+        <v>5.3799001939985602E-2</v>
       </c>
       <c r="AR3" s="1">
-        <v>0.33475583517440999</v>
-      </c>
-      <c r="AS3" s="1">
-        <v>3</v>
-      </c>
+        <v>0.90779679489277598</v>
+      </c>
+      <c r="AS3" s="1"/>
       <c r="AT3" s="1"/>
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
-      <c r="AW3" s="1"/>
-    </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>9.1371675381334231E-3</v>
-      </c>
-      <c r="B4">
-        <v>0.14430850836112119</v>
-      </c>
-      <c r="C4">
-        <v>0.13530545854146961</v>
-      </c>
-      <c r="D4">
-        <v>6.2971788711419334E-3</v>
-      </c>
-      <c r="E4">
-        <v>6.126189279720487E-3</v>
-      </c>
-      <c r="F4">
-        <v>0.15614715869026111</v>
-      </c>
-      <c r="G4">
-        <v>0.1115684790485215</v>
-      </c>
-      <c r="H4">
-        <v>0.30071057646380372</v>
-      </c>
-      <c r="I4">
-        <v>7.2295228626018032E-2</v>
-      </c>
-      <c r="J4">
-        <v>0.33783907508036398</v>
-      </c>
-      <c r="K4">
-        <v>3.8789060549769543E-2</v>
-      </c>
-      <c r="L4">
-        <v>1.6017373754903461E-2</v>
-      </c>
-      <c r="M4">
-        <v>3.1430552465091771E-2</v>
-      </c>
-      <c r="N4">
-        <v>4.7201406236839884E-3</v>
-      </c>
-      <c r="O4">
-        <v>0.5893251070040969</v>
-      </c>
-      <c r="P4">
-        <v>7.1447333262588342E-2</v>
-      </c>
-      <c r="Q4">
-        <v>9.7547666034668412E-2</v>
-      </c>
-      <c r="R4">
-        <v>5.0571564890840651E-2</v>
-      </c>
-      <c r="S4">
-        <v>1.310066759965799E-2</v>
-      </c>
-      <c r="T4">
-        <v>2.7614582902609499E-3</v>
-      </c>
-      <c r="U4">
-        <v>0.40980087130586668</v>
-      </c>
-      <c r="V4">
-        <v>0.71423330901363202</v>
-      </c>
-      <c r="W4">
-        <v>4.6456167278734438E-2</v>
-      </c>
-      <c r="X4">
-        <v>5.2393321408191862E-2</v>
-      </c>
-      <c r="Y4">
-        <v>1.8386193658974561E-2</v>
-      </c>
-      <c r="Z4">
-        <v>2.3711033233950352E-2</v>
-      </c>
-      <c r="AA4">
-        <v>0.48584596495024368</v>
-      </c>
-      <c r="AB4">
-        <v>9.5655595955882475E-4</v>
-      </c>
-      <c r="AC4">
-        <v>4.952104401205451E-2</v>
-      </c>
-      <c r="AD4">
-        <v>7.9567651250442538E-3</v>
-      </c>
-      <c r="AE4">
-        <v>2.821345853381697E-2</v>
-      </c>
-      <c r="AF4">
-        <v>5.8421429358422927E-2</v>
-      </c>
-      <c r="AG4">
-        <v>0.50799392182312297</v>
-      </c>
-      <c r="AH4">
-        <v>9.9576206096331318E-2</v>
-      </c>
-      <c r="AI4">
-        <v>5.6647139024532452E-2</v>
-      </c>
-      <c r="AJ4">
-        <v>1.840859737301718E-3</v>
-      </c>
-      <c r="AK4">
-        <v>7.9122964139277779E-5</v>
-      </c>
-      <c r="AL4">
-        <v>0.42476440717437491</v>
-      </c>
-      <c r="AM4">
-        <v>0.62882084374247182</v>
-      </c>
-      <c r="AN4">
-        <v>2.919387512413248E-2</v>
-      </c>
-      <c r="AO4">
-        <v>2.4596342074373379E-2</v>
-      </c>
-      <c r="AP4">
-        <v>2.091906334827319E-2</v>
-      </c>
-      <c r="AQ4">
-        <v>1.1202221277864591E-2</v>
-      </c>
-      <c r="AR4">
-        <v>0.2350574777549424</v>
-      </c>
-      <c r="AS4">
-        <v>4.2947152664534523</v>
-      </c>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AS4" s="1"/>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
-      <c r="AW4" s="1"/>
-    </row>
-    <row r="5" spans="1:49" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>3.3119093815730909E-2</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.11083480044112549</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2.9369699322998821E-2</v>
-      </c>
-      <c r="D5" s="2">
-        <v>7.2120950875105162E-3</v>
-      </c>
-      <c r="E5" s="2">
-        <v>8.5387337845602221E-3</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.34512412548160831</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0.61316343990228805</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0.42638340497286781</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0.68645597946322878</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.63612224356269276</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0.1475799701249762</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0.2388306267140734</v>
-      </c>
-      <c r="M5" s="2">
-        <v>9.6931620691312901E-4</v>
-      </c>
-      <c r="N5" s="2">
-        <v>1.9379373768686939E-2</v>
-      </c>
-      <c r="O5" s="2">
-        <v>0.59233749547333325</v>
-      </c>
-      <c r="P5" s="2">
-        <v>0.1314008624176258</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0.13108418294511631</v>
-      </c>
-      <c r="R5" s="2">
-        <v>0.20915858362926609</v>
-      </c>
-      <c r="S5" s="2">
-        <v>7.8910180959850251E-2</v>
-      </c>
-      <c r="T5" s="2">
-        <v>3.6437930972674851E-2</v>
-      </c>
-      <c r="U5" s="2">
-        <v>0.49262011652577897</v>
-      </c>
-      <c r="V5" s="2">
-        <v>0.59881170310497989</v>
-      </c>
-      <c r="W5" s="2">
-        <v>0.27128796022942209</v>
-      </c>
-      <c r="X5" s="2">
-        <v>0.1216232120623985</v>
-      </c>
-      <c r="Y5" s="2">
-        <v>5.9695059278267341E-2</v>
-      </c>
-      <c r="Z5" s="2">
-        <v>7.2125226840845588E-2</v>
-      </c>
-      <c r="AA5" s="2">
-        <v>0.1171585875785961</v>
-      </c>
-      <c r="AB5" s="2">
-        <v>5.0796861429136982E-2</v>
-      </c>
-      <c r="AC5" s="2">
-        <v>0.20614728477995301</v>
-      </c>
-      <c r="AD5" s="2">
-        <v>8.8304487696897915E-2</v>
-      </c>
-      <c r="AE5" s="2">
-        <v>5.506769494962746E-2</v>
-      </c>
-      <c r="AF5" s="2">
-        <v>0.30200591996311138</v>
-      </c>
-      <c r="AG5" s="2">
-        <v>0.69772607322539781</v>
-      </c>
-      <c r="AH5" s="2">
-        <v>0.12982409643590359</v>
-      </c>
-      <c r="AI5" s="2">
-        <v>0.12593300332515539</v>
-      </c>
-      <c r="AJ5" s="2">
-        <v>1.619863176268499E-3</v>
-      </c>
-      <c r="AK5" s="2">
-        <v>9.6863324001928652E-2</v>
-      </c>
-      <c r="AL5" s="2">
-        <v>0.33203758037091469</v>
-      </c>
-      <c r="AM5" s="2">
-        <v>0.38098075510332319</v>
-      </c>
-      <c r="AN5" s="2">
-        <v>0.27441392617138533</v>
-      </c>
-      <c r="AO5" s="2">
-        <v>0.234532171153542</v>
-      </c>
-      <c r="AP5" s="2">
-        <v>6.3262396939361518E-2</v>
-      </c>
-      <c r="AQ5" s="2">
-        <v>8.9154613254789392E-2</v>
-      </c>
-      <c r="AR5" s="2">
-        <v>0.59172953043968912</v>
-      </c>
-      <c r="AS5" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>3.8495447320023753E-2</v>
-      </c>
-      <c r="B6">
-        <v>2.8953733656731259E-2</v>
-      </c>
-      <c r="C6">
-        <v>1.8505355235023169E-2</v>
-      </c>
-      <c r="D6">
-        <v>7.1841749169792848E-3</v>
-      </c>
-      <c r="E6">
-        <v>1.5012566525491201E-2</v>
-      </c>
-      <c r="F6">
-        <v>0.89794130079129053</v>
-      </c>
-      <c r="G6">
-        <v>0.39550838149915718</v>
-      </c>
-      <c r="H6">
-        <v>0.87460850483452446</v>
-      </c>
-      <c r="I6">
-        <v>0.16170369551511221</v>
-      </c>
-      <c r="J6">
-        <v>0.43177986502007948</v>
-      </c>
-      <c r="K6">
-        <v>7.1541656813367077E-2</v>
-      </c>
-      <c r="L6">
-        <v>0.23650449809083779</v>
-      </c>
-      <c r="M6">
-        <v>3.073471943641637E-3</v>
-      </c>
-      <c r="N6">
-        <v>7.3187528629448634E-2</v>
-      </c>
-      <c r="O6">
-        <v>0.44008319724962019</v>
-      </c>
-      <c r="P6">
-        <v>0.20210795887203889</v>
-      </c>
-      <c r="Q6">
-        <v>0.20365209281354699</v>
-      </c>
-      <c r="R6">
-        <v>0.19611228195519451</v>
-      </c>
-      <c r="S6">
-        <v>5.251615736592459E-2</v>
-      </c>
-      <c r="T6">
-        <v>5.2204764475333537E-2</v>
-      </c>
-      <c r="U6">
-        <v>0.45525633187977621</v>
-      </c>
-      <c r="V6">
-        <v>0.69350720829699986</v>
-      </c>
-      <c r="W6">
-        <v>0.23180384300367929</v>
-      </c>
-      <c r="X6">
-        <v>0.21250301399082269</v>
-      </c>
-      <c r="Y6">
-        <v>3.6340792907377718E-2</v>
-      </c>
-      <c r="Z6">
-        <v>9.4932135800765649E-2</v>
-      </c>
-      <c r="AA6">
-        <v>0.34801959801066068</v>
-      </c>
-      <c r="AB6">
-        <v>0.17512969191275191</v>
-      </c>
-      <c r="AC6">
-        <v>0.32104608326228018</v>
-      </c>
-      <c r="AD6">
-        <v>5.1304601686309938E-2</v>
-      </c>
-      <c r="AE6">
-        <v>9.6589583842310783E-2</v>
-      </c>
-      <c r="AF6">
-        <v>0.14834693889524619</v>
-      </c>
-      <c r="AG6">
-        <v>0.35638590301472861</v>
-      </c>
-      <c r="AH6">
-        <v>4.0371061384663537E-2</v>
-      </c>
-      <c r="AI6">
-        <v>0.22808065933811639</v>
-      </c>
-      <c r="AJ6">
-        <v>3.2478540693641221E-2</v>
-      </c>
-      <c r="AK6">
-        <v>5.9984921279190667E-2</v>
-      </c>
-      <c r="AL6">
-        <v>0.46795374259354178</v>
-      </c>
-      <c r="AM6">
-        <v>0.27624809413586698</v>
-      </c>
-      <c r="AN6">
-        <v>0.16965403021739769</v>
-      </c>
-      <c r="AO6">
-        <v>5.485367006563039E-2</v>
-      </c>
-      <c r="AP6">
-        <v>9.8619744334819043E-2</v>
-      </c>
-      <c r="AQ6">
-        <v>8.7407289295625384E-2</v>
-      </c>
-      <c r="AR6">
-        <v>0.70112492268462678</v>
-      </c>
-      <c r="AS6">
-        <v>11.412542414797979</v>
-      </c>
-    </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1.860077339067754E-2</v>
-      </c>
-      <c r="B7">
-        <v>0.23950244962929079</v>
-      </c>
-      <c r="C7">
-        <v>0.63855404408750893</v>
-      </c>
-      <c r="D7">
-        <v>2.7077949635968611E-3</v>
-      </c>
-      <c r="E7">
-        <v>2.3322928784572719E-2</v>
-      </c>
-      <c r="F7">
-        <v>0.49869327828650672</v>
-      </c>
-      <c r="G7">
-        <v>0.20058372900802779</v>
-      </c>
-      <c r="H7">
-        <v>0.19554727963032531</v>
-      </c>
-      <c r="I7">
-        <v>1.8630277148478651E-3</v>
-      </c>
-      <c r="J7">
-        <v>0.89139816996806298</v>
-      </c>
-      <c r="K7">
-        <v>0.1615272795130806</v>
-      </c>
-      <c r="L7">
-        <v>0.18348451574760771</v>
-      </c>
-      <c r="M7">
-        <v>8.8102714485852898E-2</v>
-      </c>
-      <c r="N7">
-        <v>1.8619584021956469E-2</v>
-      </c>
-      <c r="O7">
-        <v>0.51254922885755771</v>
-      </c>
-      <c r="P7">
-        <v>0.35556115326258347</v>
-      </c>
-      <c r="Q7">
-        <v>5.5703744051621477E-2</v>
-      </c>
-      <c r="R7">
-        <v>2.8200445018215569E-2</v>
-      </c>
-      <c r="S7">
-        <v>4.2448392650707337E-2</v>
-      </c>
-      <c r="T7">
-        <v>1.250250946790484E-2</v>
-      </c>
-      <c r="U7">
-        <v>0.37547037060800931</v>
-      </c>
-      <c r="V7">
-        <v>0.2602225577055487</v>
-      </c>
-      <c r="W7">
-        <v>0.31694482566661147</v>
-      </c>
-      <c r="X7">
-        <v>0.26266536127273621</v>
-      </c>
-      <c r="Y7">
-        <v>7.3478267016856544E-2</v>
-      </c>
-      <c r="Z7">
-        <v>2.4095197760756169E-2</v>
-      </c>
-      <c r="AA7">
-        <v>0.70908406128901968</v>
-      </c>
-      <c r="AB7">
-        <v>0.20070306631353049</v>
-      </c>
-      <c r="AC7">
-        <v>8.9226198730497891E-2</v>
-      </c>
-      <c r="AD7">
-        <v>6.2914247306235557E-2</v>
-      </c>
-      <c r="AE7">
-        <v>6.9053699525039286E-2</v>
-      </c>
-      <c r="AF7">
-        <v>0.27294132010497901</v>
-      </c>
-      <c r="AG7">
-        <v>0.70873258955772211</v>
-      </c>
-      <c r="AH7">
-        <v>0.31250633967982749</v>
-      </c>
-      <c r="AI7">
-        <v>0.14497328686447439</v>
-      </c>
-      <c r="AJ7">
-        <v>7.87677065422311E-2</v>
-      </c>
-      <c r="AK7">
-        <v>7.4857058891397488E-2</v>
-      </c>
-      <c r="AL7">
-        <v>0.56956657654165777</v>
-      </c>
-      <c r="AM7">
-        <v>0.60821957981374142</v>
-      </c>
-      <c r="AN7">
-        <v>0.1957628361653371</v>
-      </c>
-      <c r="AO7">
-        <v>0.26824629624081342</v>
-      </c>
-      <c r="AP7">
-        <v>8.7127839743350144E-2</v>
-      </c>
-      <c r="AQ7">
-        <v>3.7556574618758443E-2</v>
-      </c>
-      <c r="AR7">
-        <v>0.61910131278436065</v>
-      </c>
-      <c r="AS7">
-        <v>12.236333278789489</v>
-      </c>
-    </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1709,24 +1157,23 @@
       <c r="AT8" s="1"/>
       <c r="AU8" s="1"/>
       <c r="AV8" s="1"/>
-      <c r="AW8" s="1"/>
     </row>
     <row r="21" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A21">
         <f>MIN(A2:A7)</f>
-        <v>3.4526878346866001E-3</v>
+        <v>9.4007123711453994E-3</v>
       </c>
       <c r="B21">
-        <f t="shared" ref="B21:AS21" si="0">MIN(B2:B7)</f>
-        <v>2.8953733656731259E-2</v>
+        <f t="shared" ref="B21:AR21" si="0">MIN(B2:B7)</f>
+        <v>0.36791989849481899</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>1.8505355235023169E-2</v>
+        <v>0.279833453987195</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>1.8670164546399999E-3</v>
+        <v>1.8670200000000001E-3</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
@@ -1734,43 +1181,43 @@
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>0.15614715869026111</v>
+        <v>0.72280092773307802</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
-        <v>0.1115684790485215</v>
+        <v>0.61098867999999995</v>
       </c>
       <c r="H21">
         <f t="shared" si="0"/>
-        <v>0.19554727963032531</v>
+        <v>0.189896295070247</v>
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
-        <v>1.8630277148478651E-3</v>
+        <v>2.7248821405216499E-2</v>
       </c>
       <c r="J21">
         <f t="shared" si="0"/>
-        <v>0.12744690276312801</v>
+        <v>0.10443477827242199</v>
       </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>3.8789060549769543E-2</v>
+        <v>2.1718387784674002E-2</v>
       </c>
       <c r="L21">
         <f t="shared" si="0"/>
-        <v>3.9906904187893E-3</v>
+        <v>3.2579912169592999E-3</v>
       </c>
       <c r="M21">
         <f t="shared" si="0"/>
-        <v>9.6931620691312901E-4</v>
+        <v>2.8500815512723501E-2</v>
       </c>
       <c r="N21">
         <f t="shared" si="0"/>
-        <v>4.7201406236839884E-3</v>
+        <v>2.6471378178950001E-2</v>
       </c>
       <c r="O21">
         <f t="shared" si="0"/>
-        <v>0.44008319724962019</v>
+        <v>0.44252004474949402</v>
       </c>
       <c r="P21">
         <f t="shared" si="0"/>
@@ -1778,11 +1225,11 @@
       </c>
       <c r="Q21">
         <f t="shared" si="0"/>
-        <v>5.5703744051621477E-2</v>
+        <v>0.17470353760207799</v>
       </c>
       <c r="R21">
         <f t="shared" si="0"/>
-        <v>2.8200445018215569E-2</v>
+        <v>7.8549897149350803E-2</v>
       </c>
       <c r="S21">
         <f t="shared" si="0"/>
@@ -1790,39 +1237,39 @@
       </c>
       <c r="T21">
         <f t="shared" si="0"/>
-        <v>2.7614582902609499E-3</v>
+        <v>9.3900620197711008E-3</v>
       </c>
       <c r="U21">
         <f t="shared" si="0"/>
-        <v>0.37547037060800931</v>
+        <v>0.41043778180456802</v>
       </c>
       <c r="V21">
         <f t="shared" si="0"/>
-        <v>0.2602225577055487</v>
+        <v>0.46669538464035898</v>
       </c>
       <c r="W21">
         <f t="shared" si="0"/>
-        <v>4.6456167278734438E-2</v>
+        <v>0.20709765999999999</v>
       </c>
       <c r="X21">
         <f t="shared" si="0"/>
-        <v>2.28364713036181E-2</v>
+        <v>7.6039620229049296E-2</v>
       </c>
       <c r="Y21">
         <f t="shared" si="0"/>
-        <v>8.7137950472754005E-3</v>
+        <v>4.67608505202751E-2</v>
       </c>
       <c r="Z21">
         <f t="shared" si="0"/>
-        <v>2.3711033233950352E-2</v>
+        <v>4.1980710199390897E-2</v>
       </c>
       <c r="AA21">
         <f t="shared" si="0"/>
-        <v>0.1171585875785961</v>
+        <v>0.42496023035477798</v>
       </c>
       <c r="AB21">
         <f t="shared" si="0"/>
-        <v>9.5655595955882475E-4</v>
+        <v>5.6174209245325499E-2</v>
       </c>
       <c r="AC21">
         <f t="shared" si="0"/>
@@ -1830,15 +1277,15 @@
       </c>
       <c r="AD21">
         <f t="shared" si="0"/>
-        <v>7.9567651250442538E-3</v>
+        <v>1.2356657523411699E-2</v>
       </c>
       <c r="AE21">
         <f t="shared" si="0"/>
-        <v>2.821345853381697E-2</v>
+        <v>2.7184729575304101E-2</v>
       </c>
       <c r="AF21">
         <f t="shared" si="0"/>
-        <v>5.8421429358422927E-2</v>
+        <v>0.115646764697444</v>
       </c>
       <c r="AG21">
         <f t="shared" si="0"/>
@@ -1846,23 +1293,23 @@
       </c>
       <c r="AH21">
         <f t="shared" si="0"/>
-        <v>6.5757563076245E-3</v>
+        <v>1.1418786832505299E-2</v>
       </c>
       <c r="AI21">
         <f t="shared" si="0"/>
-        <v>5.6647139024532452E-2</v>
+        <v>0.15919674569310299</v>
       </c>
       <c r="AJ21">
         <f t="shared" si="0"/>
-        <v>1.619863176268499E-3</v>
+        <v>1.11678579741689E-2</v>
       </c>
       <c r="AK21">
         <f t="shared" si="0"/>
-        <v>7.9122964139277779E-5</v>
+        <v>5.7276742831977499E-2</v>
       </c>
       <c r="AL21">
         <f t="shared" si="0"/>
-        <v>0.19198668795559201</v>
+        <v>0.18369111088983001</v>
       </c>
       <c r="AM21">
         <f t="shared" si="0"/>
@@ -1870,53 +1317,53 @@
       </c>
       <c r="AN21">
         <f t="shared" si="0"/>
-        <v>2.919387512413248E-2</v>
+        <v>0.25280292919952702</v>
       </c>
       <c r="AO21">
         <f t="shared" si="0"/>
-        <v>2.4596342074373379E-2</v>
+        <v>0.26215336739706802</v>
       </c>
       <c r="AP21">
         <f t="shared" si="0"/>
-        <v>2.091906334827319E-2</v>
+        <v>5.04783859417232E-2</v>
       </c>
       <c r="AQ21">
         <f t="shared" si="0"/>
-        <v>1.1202221277864591E-2</v>
+        <v>3.8138699248282497E-2</v>
       </c>
       <c r="AR21">
         <f t="shared" si="0"/>
-        <v>0.2350574777549424</v>
+        <v>0.33475583517440999</v>
       </c>
     </row>
     <row r="22" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A22">
         <f>MAX(A2:A7)</f>
-        <v>3.8495447320023753E-2</v>
+        <v>2.07306177012637E-2</v>
       </c>
       <c r="B22">
-        <f t="shared" ref="B22:AS22" si="1">MAX(B2:B7)</f>
-        <v>0.63487402101185697</v>
+        <f t="shared" ref="B22:AR22" si="1">MAX(B2:B7)</f>
+        <v>0.46281241145402002</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>0.63855404408750893</v>
+        <v>0.97708446480051203</v>
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
-        <v>7.2120950875105162E-3</v>
+        <v>5.9498199999999998E-3</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
-        <v>2.3322928784572719E-2</v>
+        <v>9.9136523316660004E-3</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>0.89794130079129053</v>
+        <v>0.81766665355022605</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>0.83705726579801099</v>
+        <v>0.83705726999999996</v>
       </c>
       <c r="H22">
         <f t="shared" si="1"/>
@@ -1924,27 +1371,27 @@
       </c>
       <c r="I22">
         <f t="shared" si="1"/>
-        <v>0.68645597946322878</v>
+        <v>8.2915355481762196E-2</v>
       </c>
       <c r="J22">
         <f t="shared" si="1"/>
-        <v>0.89139816996806298</v>
+        <v>0.12744690276312801</v>
       </c>
       <c r="K22">
         <f t="shared" si="1"/>
-        <v>0.30884647216498001</v>
+        <v>0.19678865195313899</v>
       </c>
       <c r="L22">
         <f t="shared" si="1"/>
-        <v>0.2388306267140734</v>
+        <v>1.5923241139799298E-2</v>
       </c>
       <c r="M22">
         <f t="shared" si="1"/>
-        <v>8.8102714485852898E-2</v>
+        <v>5.4910744572851701E-2</v>
       </c>
       <c r="N22">
         <f t="shared" si="1"/>
-        <v>9.1426731560706395E-2</v>
+        <v>3.0458041765055899E-2</v>
       </c>
       <c r="O22">
         <f t="shared" si="1"/>
@@ -1952,27 +1399,27 @@
       </c>
       <c r="P22">
         <f t="shared" si="1"/>
-        <v>0.97084189112677</v>
+        <v>0.70921771659038502</v>
       </c>
       <c r="Q22">
         <f t="shared" si="1"/>
-        <v>0.20365209281354699</v>
+        <v>0.32178463746241998</v>
       </c>
       <c r="R22">
         <f t="shared" si="1"/>
-        <v>0.20915858362926609</v>
+        <v>0.18075157117934901</v>
       </c>
       <c r="S22">
         <f t="shared" si="1"/>
-        <v>7.8910180959850251E-2</v>
+        <v>1.82360276804681E-2</v>
       </c>
       <c r="T22">
         <f t="shared" si="1"/>
-        <v>9.1620661165299502E-2</v>
+        <v>8.5698109252469595E-2</v>
       </c>
       <c r="U22">
         <f t="shared" si="1"/>
-        <v>0.51255313256903301</v>
+        <v>0.731290194609307</v>
       </c>
       <c r="V22">
         <f t="shared" si="1"/>
@@ -1980,7 +1427,7 @@
       </c>
       <c r="W22">
         <f t="shared" si="1"/>
-        <v>0.31694482566661147</v>
+        <v>0.23421243999999999</v>
       </c>
       <c r="X22">
         <f t="shared" si="1"/>
@@ -1988,67 +1435,67 @@
       </c>
       <c r="Y22">
         <f t="shared" si="1"/>
-        <v>7.3478267016856544E-2</v>
+        <v>7.2353529170675404E-2</v>
       </c>
       <c r="Z22">
         <f t="shared" si="1"/>
-        <v>9.4932135800765649E-2</v>
+        <v>5.8604597107539597E-2</v>
       </c>
       <c r="AA22">
         <f t="shared" si="1"/>
-        <v>0.72693454033265903</v>
+        <v>0.77126681168856404</v>
       </c>
       <c r="AB22">
         <f t="shared" si="1"/>
-        <v>0.20270858100195199</v>
+        <v>0.110805698091791</v>
       </c>
       <c r="AC22">
         <f t="shared" si="1"/>
-        <v>0.32104608326228018</v>
+        <v>3.81399365882392E-2</v>
       </c>
       <c r="AD22">
         <f t="shared" si="1"/>
-        <v>8.8304487696897915E-2</v>
+        <v>8.0036166686743307E-2</v>
       </c>
       <c r="AE22">
         <f t="shared" si="1"/>
-        <v>9.6589583842310783E-2</v>
+        <v>3.7052656274977898E-2</v>
       </c>
       <c r="AF22">
         <f t="shared" si="1"/>
-        <v>0.30200591996311138</v>
+        <v>0.338475915628696</v>
       </c>
       <c r="AG22">
         <f t="shared" si="1"/>
-        <v>0.70873258955772211</v>
+        <v>0.78227418302001295</v>
       </c>
       <c r="AH22">
         <f t="shared" si="1"/>
-        <v>0.31250633967982749</v>
+        <v>0.118696637821815</v>
       </c>
       <c r="AI22">
         <f t="shared" si="1"/>
-        <v>0.22808065933811639</v>
+        <v>0.21766613578879801</v>
       </c>
       <c r="AJ22">
         <f t="shared" si="1"/>
-        <v>7.87677065422311E-2</v>
+        <v>3.6664634935266401E-2</v>
       </c>
       <c r="AK22">
         <f t="shared" si="1"/>
-        <v>9.6863324001928652E-2</v>
+        <v>8.7221565121345199E-2</v>
       </c>
       <c r="AL22">
         <f t="shared" si="1"/>
-        <v>0.56956657654165777</v>
+        <v>0.34933321383960902</v>
       </c>
       <c r="AM22">
         <f t="shared" si="1"/>
-        <v>0.63217241092265097</v>
+        <v>0.992363144426335</v>
       </c>
       <c r="AN22">
         <f t="shared" si="1"/>
-        <v>0.27441392617138533</v>
+        <v>0.28925486566592901</v>
       </c>
       <c r="AO22">
         <f t="shared" si="1"/>
@@ -2056,15 +1503,15 @@
       </c>
       <c r="AP22">
         <f t="shared" si="1"/>
-        <v>9.8619744334819043E-2</v>
+        <v>6.9184246677001696E-2</v>
       </c>
       <c r="AQ22">
         <f t="shared" si="1"/>
-        <v>9.2471551226675899E-2</v>
+        <v>5.3799001939985602E-2</v>
       </c>
       <c r="AR22">
         <f t="shared" si="1"/>
-        <v>0.75948171815090304</v>
+        <v>0.90779679489277598</v>
       </c>
     </row>
   </sheetData>
@@ -2074,285 +1521,305 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D565706-8B0A-7149-B0A3-5E68A8A9D30C}">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <f>A3+1</f>
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="2"/>
+      <c r="D4" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <f t="shared" ref="A5:A68" si="0">A4+1</f>
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="2"/>
+      <c r="D5" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3"/>
+      <c r="D6" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3"/>
+      <c r="D7" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3"/>
+      <c r="D8" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3"/>
+      <c r="D9" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3"/>
+      <c r="D10" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3"/>
+      <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3"/>
+      <c r="D12" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3"/>
+      <c r="D13" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3"/>
+      <c r="D14" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3"/>
+      <c r="D15" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3"/>
+      <c r="D16" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3"/>
+      <c r="D17" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3"/>
+      <c r="D18" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3"/>
+      <c r="D19" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3"/>
+      <c r="D20" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="3"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="3"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="3"/>
+      <c r="D23" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3"/>
+      <c r="D24" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3"/>
+      <c r="D25" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B27" s="3"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="3"/>
+      <c r="D28" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>32</v>

</xml_diff>

<commit_message>
added ODE 100 PS landscape
</commit_message>
<xml_diff>
--- a/optimizer_outputs_resilience.xlsx
+++ b/optimizer_outputs_resilience.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilyneil/Desktop/rewilding_resilience/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DB265B-56BA-8F4C-913D-D11FC5691F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE116222-3CDE-C649-AD71-1171A51A280A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="500" windowWidth="19120" windowHeight="16560" xr2:uid="{AE1BBF2D-EC41-B34F-81BF-523AF052BB25}"/>
+    <workbookView xWindow="7840" yWindow="500" windowWidth="20960" windowHeight="16560" xr2:uid="{AE1BBF2D-EC41-B34F-81BF-523AF052BB25}"/>
   </bookViews>
   <sheets>
     <sheet name="outputs" sheetId="1" r:id="rId1"/>
@@ -427,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -448,6 +448,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -762,11 +763,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D6EFC4-B0D4-EA49-B8BA-BDB3C827D59C}">
-  <dimension ref="A1:AU108"/>
+  <dimension ref="A1:AU105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AX63" sqref="AX63"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AT17" sqref="AT17:AT27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1047,7 +1048,7 @@
       <c r="AS2">
         <v>1.1074691591477459</v>
       </c>
-      <c r="AT2" s="2">
+      <c r="AT2" s="10">
         <v>1</v>
       </c>
     </row>
@@ -1187,8 +1188,8 @@
       <c r="AS3">
         <v>1.232019943912855</v>
       </c>
-      <c r="AT3" s="9">
-        <f t="shared" ref="AT3:AT104" si="0">AT2+1</f>
+      <c r="AT3" s="10">
+        <f>AT2+1</f>
         <v>2</v>
       </c>
     </row>
@@ -1328,8 +1329,8 @@
       <c r="AS4">
         <v>1.465617557529735</v>
       </c>
-      <c r="AT4" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT4" s="10">
+        <f t="shared" ref="AT4:AT67" si="0">AT3+1</f>
         <v>3</v>
       </c>
     </row>
@@ -1469,7 +1470,7 @@
       <c r="AS5">
         <v>2.0138454812143971</v>
       </c>
-      <c r="AT5" s="9">
+      <c r="AT5" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1610,7 +1611,7 @@
       <c r="AS6">
         <v>2.1039387991197018</v>
       </c>
-      <c r="AT6" s="9">
+      <c r="AT6" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1751,7 +1752,7 @@
       <c r="AS7">
         <v>2.201385941770551</v>
       </c>
-      <c r="AT7" s="9">
+      <c r="AT7" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1892,7 +1893,7 @@
       <c r="AS8">
         <v>2.5113215145204628</v>
       </c>
-      <c r="AT8" s="9">
+      <c r="AT8" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -2033,8 +2034,8 @@
       <c r="AS9">
         <v>2.8011633355828551</v>
       </c>
-      <c r="AT9" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT9" s="10">
+        <f>AT8+1</f>
         <v>8</v>
       </c>
     </row>
@@ -2174,7 +2175,7 @@
       <c r="AS10">
         <v>2.9360972680986781</v>
       </c>
-      <c r="AT10" s="9">
+      <c r="AT10" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -2315,7 +2316,7 @@
       <c r="AS11" s="1">
         <v>3</v>
       </c>
-      <c r="AT11" s="9">
+      <c r="AT11" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -2456,7 +2457,7 @@
       <c r="AS12">
         <v>3.1607936088315149</v>
       </c>
-      <c r="AT12" s="9">
+      <c r="AT12" s="10">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -2597,7 +2598,7 @@
       <c r="AS13">
         <v>3.2223036293150211</v>
       </c>
-      <c r="AT13" s="9">
+      <c r="AT13" s="10">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2738,7 +2739,7 @@
       <c r="AS14">
         <v>3.4206445259211629</v>
       </c>
-      <c r="AT14" s="9">
+      <c r="AT14" s="10">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2879,7 +2880,7 @@
       <c r="AS15">
         <v>3.4782601349659119</v>
       </c>
-      <c r="AT15" s="9">
+      <c r="AT15" s="10">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -3020,7 +3021,7 @@
       <c r="AS16">
         <v>3.5445993654228931</v>
       </c>
-      <c r="AT16" s="9">
+      <c r="AT16" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -3161,7 +3162,7 @@
       <c r="AS17">
         <v>3.63678960763127</v>
       </c>
-      <c r="AT17" s="9">
+      <c r="AT17" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -3302,7 +3303,7 @@
       <c r="AS18">
         <v>3.8570078287385838</v>
       </c>
-      <c r="AT18" s="9">
+      <c r="AT18" s="10">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -3444,7 +3445,7 @@
       <c r="AS19">
         <v>4.0981538041161567</v>
       </c>
-      <c r="AT19" s="9">
+      <c r="AT19" s="10">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -3585,7 +3586,7 @@
       <c r="AS20">
         <v>4.1789900287888049</v>
       </c>
-      <c r="AT20" s="9">
+      <c r="AT20" s="10">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -3726,7 +3727,7 @@
       <c r="AS21">
         <v>4.3696633330573924</v>
       </c>
-      <c r="AT21" s="9">
+      <c r="AT21" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -3867,7 +3868,7 @@
       <c r="AS22">
         <v>4.4225300464552513</v>
       </c>
-      <c r="AT22" s="9">
+      <c r="AT22" s="10">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -4008,7 +4009,7 @@
       <c r="AS23">
         <v>4.6639270944633946</v>
       </c>
-      <c r="AT23" s="9">
+      <c r="AT23" s="10">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
@@ -4149,7 +4150,7 @@
       <c r="AS24">
         <v>4.7262040736240252</v>
       </c>
-      <c r="AT24" s="9">
+      <c r="AT24" s="10">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
@@ -4290,7 +4291,7 @@
       <c r="AS25">
         <v>4.9091693032499091</v>
       </c>
-      <c r="AT25" s="9">
+      <c r="AT25" s="10">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
@@ -4431,7 +4432,7 @@
       <c r="AS26">
         <v>5.1330241113395019</v>
       </c>
-      <c r="AT26" s="9">
+      <c r="AT26" s="10">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
@@ -4572,7 +4573,7 @@
       <c r="AS27">
         <v>5.2212427909568682</v>
       </c>
-      <c r="AT27" s="9">
+      <c r="AT27" s="10">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
@@ -4713,7 +4714,7 @@
       <c r="AS28">
         <v>5.364284256993221</v>
       </c>
-      <c r="AT28" s="9">
+      <c r="AT28" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
@@ -4854,7 +4855,7 @@
       <c r="AS29">
         <v>5.4768946830110963</v>
       </c>
-      <c r="AT29" s="9">
+      <c r="AT29" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
@@ -4995,7 +4996,7 @@
       <c r="AS30">
         <v>6.2883888404253607</v>
       </c>
-      <c r="AT30" s="9">
+      <c r="AT30" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
@@ -5136,7 +5137,7 @@
       <c r="AS31">
         <v>6.3052775948044326</v>
       </c>
-      <c r="AT31" s="9">
+      <c r="AT31" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -5277,7 +5278,7 @@
       <c r="AS32">
         <v>6.617539307764237</v>
       </c>
-      <c r="AT32" s="9">
+      <c r="AT32" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
@@ -5419,7 +5420,7 @@
       <c r="AS33">
         <v>6.6420750230955923</v>
       </c>
-      <c r="AT33" s="9">
+      <c r="AT33" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
@@ -5560,7 +5561,7 @@
       <c r="AS34">
         <v>6.694011840792065</v>
       </c>
-      <c r="AT34" s="9">
+      <c r="AT34" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
@@ -5701,7 +5702,7 @@
       <c r="AS35">
         <v>6.8425625212301808</v>
       </c>
-      <c r="AT35" s="9">
+      <c r="AT35" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
@@ -5842,7 +5843,7 @@
       <c r="AS36">
         <v>7.1760686749920133</v>
       </c>
-      <c r="AT36" s="9">
+      <c r="AT36" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -5983,7 +5984,7 @@
       <c r="AS37">
         <v>7.42703986382379</v>
       </c>
-      <c r="AT37" s="9">
+      <c r="AT37" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
@@ -6124,7 +6125,7 @@
       <c r="AS38">
         <v>7.705129221695592</v>
       </c>
-      <c r="AT38" s="9">
+      <c r="AT38" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
@@ -6265,7 +6266,7 @@
       <c r="AS39">
         <v>7.9912111557681094</v>
       </c>
-      <c r="AT39" s="9">
+      <c r="AT39" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
@@ -6406,7 +6407,7 @@
       <c r="AS40">
         <v>8.453945087038969</v>
       </c>
-      <c r="AT40" s="9">
+      <c r="AT40" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
@@ -6547,7 +6548,7 @@
       <c r="AS41">
         <v>8.5466908222529003</v>
       </c>
-      <c r="AT41" s="9">
+      <c r="AT41" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
@@ -6688,1842 +6689,1840 @@
       <c r="AS42">
         <v>8.7213212721891136</v>
       </c>
-      <c r="AT42" s="9">
+      <c r="AT42" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>4.5032232149025242E-2</v>
+        <v>5.5844377207507567E-2</v>
       </c>
       <c r="B43">
-        <v>0.42130540448817372</v>
+        <v>0.503175130328403</v>
       </c>
       <c r="C43">
-        <v>1.5042004789833641E-3</v>
+        <v>5.5064809516272351E-2</v>
       </c>
       <c r="D43">
-        <v>3.4442819755635149E-3</v>
+        <v>3.2229557205766101E-3</v>
       </c>
       <c r="E43">
-        <v>3.2642681969731911E-3</v>
+        <v>8.29720971744515E-3</v>
       </c>
       <c r="F43">
-        <v>0.85763408963719934</v>
+        <v>8.2650958801349872E-2</v>
       </c>
       <c r="G43">
-        <v>0.53134492302811165</v>
+        <v>4.9392056315933019E-2</v>
       </c>
       <c r="H43">
-        <v>0.53300496190756097</v>
+        <v>0.7624556266160526</v>
       </c>
       <c r="I43">
-        <v>0.2337694362537944</v>
+        <v>0.1168264058934458</v>
       </c>
       <c r="J43">
-        <v>0.1931661575895994</v>
+        <v>0.1123120270678927</v>
       </c>
       <c r="K43">
-        <v>2.536062908048807E-2</v>
+        <v>3.9954616196046358E-2</v>
       </c>
       <c r="L43">
-        <v>4.8434941510187263E-2</v>
+        <v>4.3571573557869576E-3</v>
       </c>
       <c r="M43">
-        <v>6.5694198234562493E-3</v>
+        <v>1.9543039782162371E-2</v>
       </c>
       <c r="N43">
-        <v>1.6734627965114879E-2</v>
+        <v>5.0043624961356977E-3</v>
       </c>
       <c r="O43">
-        <v>0.37843867993073071</v>
+        <v>0.71128040425545369</v>
       </c>
       <c r="P43">
-        <v>0.16001156366890229</v>
+        <v>4.3148453092102662E-2</v>
       </c>
       <c r="Q43">
-        <v>3.2263273036647611E-2</v>
+        <v>4.0472975299321416E-3</v>
       </c>
       <c r="R43">
-        <v>8.2099616536140479E-2</v>
+        <v>5.6918194818985877E-2</v>
       </c>
       <c r="S43">
-        <v>6.4244571146057086E-4</v>
+        <v>1.9841914075179091E-2</v>
       </c>
       <c r="T43">
-        <v>4.3711090227794213E-3</v>
+        <v>9.4732358641126256E-4</v>
       </c>
       <c r="U43">
-        <v>0.33885521978127159</v>
+        <v>0.55073033758411238</v>
       </c>
       <c r="V43">
-        <v>1.8936358108400941E-2</v>
+        <v>0.22903645390231611</v>
       </c>
       <c r="W43">
-        <v>5.0025572936980317E-2</v>
+        <v>7.0579491654722798E-2</v>
       </c>
       <c r="X43">
-        <v>7.9536510904042484E-2</v>
+        <v>3.8240897233239681E-3</v>
       </c>
       <c r="Y43">
-        <v>1.112182289916723E-2</v>
+        <v>8.1411771694513222E-3</v>
       </c>
       <c r="Z43">
-        <v>1.4101540565114449E-2</v>
+        <v>2.320012535825218E-2</v>
       </c>
       <c r="AA43">
-        <v>0.2437279277374739</v>
+        <v>9.390290696203013E-2</v>
       </c>
       <c r="AB43">
-        <v>3.8111250151659309E-2</v>
+        <v>7.8640078510147177E-2</v>
       </c>
       <c r="AC43">
-        <v>1.1009040237550829E-2</v>
+        <v>2.985745315608565E-2</v>
       </c>
       <c r="AD43">
-        <v>1.018513007291866E-2</v>
+        <v>2.2661074742762959E-2</v>
       </c>
       <c r="AE43">
-        <v>2.0910678407008009E-2</v>
+        <v>1.46591185778201E-2</v>
       </c>
       <c r="AF43">
-        <v>0.34923724430395747</v>
+        <v>0.37761765811416448</v>
       </c>
       <c r="AG43">
-        <v>0.22766970001946399</v>
+        <v>0.21966034711588031</v>
       </c>
       <c r="AH43">
-        <v>3.9255227805494827E-2</v>
+        <v>5.1981239955235112E-2</v>
       </c>
       <c r="AI43">
-        <v>4.4767301931991903E-2</v>
+        <v>8.1538703924007375E-2</v>
       </c>
       <c r="AJ43">
-        <v>1.278912308499534E-2</v>
+        <v>1.4828007658941451E-2</v>
       </c>
       <c r="AK43">
-        <v>2.1165711646610411E-2</v>
+        <v>1.636409570599914E-3</v>
       </c>
       <c r="AL43">
-        <v>0.53110957174559303</v>
+        <v>0.44971432669268852</v>
       </c>
       <c r="AM43">
-        <v>5.7837323332354112E-2</v>
+        <v>0.2302259582435971</v>
       </c>
       <c r="AN43">
-        <v>5.7849717250085801E-2</v>
+        <v>4.4457620391665613E-2</v>
       </c>
       <c r="AO43">
-        <v>7.5983906591731945E-2</v>
+        <v>8.067362373168678E-2</v>
       </c>
       <c r="AP43">
-        <v>8.4507322311617779E-3</v>
+        <v>2.7970395440560492E-3</v>
       </c>
       <c r="AQ43">
-        <v>1.6930935743566931E-2</v>
+        <v>2.2795106291409961E-2</v>
       </c>
       <c r="AR43">
-        <v>6.6240538801130344E-2</v>
+        <v>9.2893313035505742E-2</v>
       </c>
       <c r="AS43">
-        <v>9.22623545496924</v>
-      </c>
-      <c r="AT43" s="9">
+        <v>9.2185638650729427</v>
+      </c>
+      <c r="AT43" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>6.4329201851894044E-2</v>
+        <v>4.5032232149025242E-2</v>
       </c>
       <c r="B44">
-        <v>0.79198324954313548</v>
+        <v>0.42130540448817372</v>
       </c>
       <c r="C44">
-        <v>0.13654661242337349</v>
+        <v>1.5042004789833641E-3</v>
       </c>
       <c r="D44">
-        <v>4.1630438355298553E-3</v>
+        <v>3.4442819755635149E-3</v>
       </c>
       <c r="E44">
-        <v>4.724371378722384E-3</v>
+        <v>3.2642681969731911E-3</v>
       </c>
       <c r="F44">
-        <v>0.59752975750207082</v>
+        <v>0.85763408963719934</v>
       </c>
       <c r="G44">
-        <v>0.7656068920847916</v>
+        <v>0.53134492302811165</v>
       </c>
       <c r="H44">
-        <v>0.27817404589688022</v>
+        <v>0.53300496190756097</v>
       </c>
       <c r="I44">
-        <v>0.1012062578961173</v>
+        <v>0.2337694362537944</v>
       </c>
       <c r="J44">
-        <v>3.8736106797249537E-2</v>
+        <v>0.1931661575895994</v>
       </c>
       <c r="K44">
-        <v>7.4193178191072809E-2</v>
+        <v>2.536062908048807E-2</v>
       </c>
       <c r="L44">
-        <v>2.048269319152974E-2</v>
+        <v>4.8434941510187263E-2</v>
       </c>
       <c r="M44">
-        <v>1.4620370825232249E-2</v>
+        <v>6.5694198234562493E-3</v>
       </c>
       <c r="N44">
-        <v>2.6894652734071709E-3</v>
+        <v>1.6734627965114879E-2</v>
       </c>
       <c r="O44">
-        <v>0.71288308714835247</v>
+        <v>0.37843867993073071</v>
       </c>
       <c r="P44">
-        <v>0.20062469781956629</v>
+        <v>0.16001156366890229</v>
       </c>
       <c r="Q44">
-        <v>1.1576587065603159E-3</v>
+        <v>3.2263273036647611E-2</v>
       </c>
       <c r="R44">
-        <v>4.1297068451133567E-2</v>
+        <v>8.2099616536140479E-2</v>
       </c>
       <c r="S44">
-        <v>1.9715265073969101E-2</v>
+        <v>6.4244571146057086E-4</v>
       </c>
       <c r="T44">
-        <v>1.8169681739827609E-2</v>
+        <v>4.3711090227794213E-3</v>
       </c>
       <c r="U44">
-        <v>0.33518483908119578</v>
+        <v>0.33885521978127159</v>
       </c>
       <c r="V44">
-        <v>5.7905882517308882E-2</v>
+        <v>1.8936358108400941E-2</v>
       </c>
       <c r="W44">
-        <v>6.8953389286236608E-2</v>
+        <v>5.0025572936980317E-2</v>
       </c>
       <c r="X44">
-        <v>1.100439315467344E-2</v>
+        <v>7.9536510904042484E-2</v>
       </c>
       <c r="Y44">
-        <v>1.347533721072983E-2</v>
+        <v>1.112182289916723E-2</v>
       </c>
       <c r="Z44">
-        <v>1.774586946093519E-2</v>
+        <v>1.4101540565114449E-2</v>
       </c>
       <c r="AA44">
-        <v>0.1815242402263833</v>
+        <v>0.2437279277374739</v>
       </c>
       <c r="AB44">
-        <v>2.6902329735890629E-2</v>
+        <v>3.8111250151659309E-2</v>
       </c>
       <c r="AC44">
-        <v>6.1989181802847883E-2</v>
+        <v>1.1009040237550829E-2</v>
       </c>
       <c r="AD44">
-        <v>5.8346282578038934E-3</v>
+        <v>1.018513007291866E-2</v>
       </c>
       <c r="AE44">
-        <v>5.0094150593403249E-3</v>
+        <v>2.0910678407008009E-2</v>
       </c>
       <c r="AF44">
-        <v>1.4816318222834021E-2</v>
+        <v>0.34923724430395747</v>
       </c>
       <c r="AG44">
-        <v>0.16670565951531691</v>
+        <v>0.22766970001946399</v>
       </c>
       <c r="AH44">
-        <v>7.4049778918650097E-2</v>
+        <v>3.9255227805494827E-2</v>
       </c>
       <c r="AI44">
-        <v>2.7266086349593009E-2</v>
+        <v>4.4767301931991903E-2</v>
       </c>
       <c r="AJ44">
-        <v>1.2942650063514589E-2</v>
+        <v>1.278912308499534E-2</v>
       </c>
       <c r="AK44">
-        <v>8.1705794982600641E-3</v>
+        <v>2.1165711646610411E-2</v>
       </c>
       <c r="AL44">
-        <v>0.15714611952515481</v>
+        <v>0.53110957174559303</v>
       </c>
       <c r="AM44">
-        <v>0.2409933599251782</v>
+        <v>5.7837323332354112E-2</v>
       </c>
       <c r="AN44">
-        <v>3.5672398222948848E-2</v>
+        <v>5.7849717250085801E-2</v>
       </c>
       <c r="AO44">
-        <v>8.1814260101723772E-3</v>
+        <v>7.5983906591731945E-2</v>
       </c>
       <c r="AP44">
-        <v>8.2837290787503466E-3</v>
+        <v>8.4507322311617779E-3</v>
       </c>
       <c r="AQ44">
-        <v>1.3541643311777631E-2</v>
+        <v>1.6930935743566931E-2</v>
       </c>
       <c r="AR44">
-        <v>0.72020190195718747</v>
+        <v>6.6240538801130344E-2</v>
       </c>
       <c r="AS44">
-        <v>9.8466839404525253</v>
-      </c>
-      <c r="AT44" s="9">
+        <v>9.22623545496924</v>
+      </c>
+      <c r="AT44" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>4.9443383935648171E-2</v>
+        <v>6.4329201851894044E-2</v>
       </c>
       <c r="B45">
-        <v>0.51395299488965107</v>
+        <v>0.79198324954313548</v>
       </c>
       <c r="C45">
-        <v>2.0659651624071681E-2</v>
+        <v>0.13654661242337349</v>
       </c>
       <c r="D45">
-        <v>7.0569576486078471E-3</v>
+        <v>4.1630438355298553E-3</v>
       </c>
       <c r="E45">
-        <v>5.274003385786429E-3</v>
+        <v>4.724371378722384E-3</v>
       </c>
       <c r="F45">
-        <v>0.46955139287930042</v>
+        <v>0.59752975750207082</v>
       </c>
       <c r="G45">
-        <v>0.83480001109334045</v>
+        <v>0.7656068920847916</v>
       </c>
       <c r="H45">
-        <v>0.90757486346015837</v>
+        <v>0.27817404589688022</v>
       </c>
       <c r="I45">
-        <v>0.31219539684782882</v>
+        <v>0.1012062578961173</v>
       </c>
       <c r="J45">
-        <v>0.16892612548419861</v>
+        <v>3.8736106797249537E-2</v>
       </c>
       <c r="K45">
-        <v>6.1147837696696548E-3</v>
+        <v>7.4193178191072809E-2</v>
       </c>
       <c r="L45">
-        <v>3.375625099569092E-2</v>
+        <v>2.048269319152974E-2</v>
       </c>
       <c r="M45">
-        <v>7.4817077918721223E-3</v>
+        <v>1.4620370825232249E-2</v>
       </c>
       <c r="N45">
-        <v>5.4018893943401404E-3</v>
+        <v>2.6894652734071709E-3</v>
       </c>
       <c r="O45">
-        <v>0.57768263910821394</v>
+        <v>0.71288308714835247</v>
       </c>
       <c r="P45">
-        <v>0.14025502316821489</v>
+        <v>0.20062469781956629</v>
       </c>
       <c r="Q45">
-        <v>7.935327201746209E-2</v>
+        <v>1.1576587065603159E-3</v>
       </c>
       <c r="R45">
-        <v>4.3508783003021613E-2</v>
+        <v>4.1297068451133567E-2</v>
       </c>
       <c r="S45">
-        <v>1.456762742781907E-2</v>
+        <v>1.9715265073969101E-2</v>
       </c>
       <c r="T45">
-        <v>8.8941340366296504E-3</v>
+        <v>1.8169681739827609E-2</v>
       </c>
       <c r="U45">
-        <v>0.66085633100902896</v>
+        <v>0.33518483908119578</v>
       </c>
       <c r="V45">
-        <v>0.21463159089297601</v>
+        <v>5.7905882517308882E-2</v>
       </c>
       <c r="W45">
-        <v>1.7539373203283099E-2</v>
+        <v>6.8953389286236608E-2</v>
       </c>
       <c r="X45">
-        <v>7.4281091526034904E-2</v>
+        <v>1.100439315467344E-2</v>
       </c>
       <c r="Y45">
-        <v>1.474569988889079E-2</v>
+        <v>1.347533721072983E-2</v>
       </c>
       <c r="Z45">
-        <v>1.012301033191672E-3</v>
+        <v>1.774586946093519E-2</v>
       </c>
       <c r="AA45">
-        <v>0.12739657930233689</v>
+        <v>0.1815242402263833</v>
       </c>
       <c r="AB45">
-        <v>6.8236778265022391E-2</v>
+        <v>2.6902329735890629E-2</v>
       </c>
       <c r="AC45">
-        <v>5.3770575819476238E-2</v>
+        <v>6.1989181802847883E-2</v>
       </c>
       <c r="AD45">
-        <v>2.342551983058613E-2</v>
+        <v>5.8346282578038934E-3</v>
       </c>
       <c r="AE45">
-        <v>2.7674092456965618E-3</v>
+        <v>5.0094150593403249E-3</v>
       </c>
       <c r="AF45">
-        <v>0.3458131795668517</v>
+        <v>1.4816318222834021E-2</v>
       </c>
       <c r="AG45">
-        <v>0.1065037626602537</v>
+        <v>0.16670565951531691</v>
       </c>
       <c r="AH45">
-        <v>2.4276531711530939E-2</v>
+        <v>7.4049778918650097E-2</v>
       </c>
       <c r="AI45">
-        <v>2.0619216030688631E-2</v>
+        <v>2.7266086349593009E-2</v>
       </c>
       <c r="AJ45">
-        <v>1.352460619641766E-2</v>
+        <v>1.2942650063514589E-2</v>
       </c>
       <c r="AK45">
-        <v>2.017793122889746E-2</v>
+        <v>8.1705794982600641E-3</v>
       </c>
       <c r="AL45">
-        <v>0.6830934981814103</v>
+        <v>0.15714611952515481</v>
       </c>
       <c r="AM45">
-        <v>0.17420007605503829</v>
+        <v>0.2409933599251782</v>
       </c>
       <c r="AN45">
-        <v>1.241437225539291E-2</v>
+        <v>3.5672398222948848E-2</v>
       </c>
       <c r="AO45">
-        <v>7.0725758446066656E-2</v>
+        <v>8.1814260101723772E-3</v>
       </c>
       <c r="AP45">
-        <v>7.0860193317136251E-3</v>
+        <v>8.2837290787503466E-3</v>
       </c>
       <c r="AQ45">
-        <v>1.1895785505552431E-2</v>
+        <v>1.3541643311777631E-2</v>
       </c>
       <c r="AR45">
-        <v>0.63693508260260046</v>
+        <v>0.72020190195718747</v>
       </c>
       <c r="AS45">
-        <v>12.211819053800459</v>
-      </c>
-      <c r="AT45" s="9">
+        <v>9.8466839404525253</v>
+      </c>
+      <c r="AT45" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>0.14569228678046861</v>
+        <v>4.9443383935648171E-2</v>
       </c>
       <c r="B46">
-        <v>0.16444242211683149</v>
+        <v>0.51395299488965107</v>
       </c>
       <c r="C46">
-        <v>0.46019856612543247</v>
+        <v>2.0659651624071681E-2</v>
       </c>
       <c r="D46">
-        <v>2.0657172461282388E-3</v>
+        <v>7.0569576486078471E-3</v>
       </c>
       <c r="E46">
-        <v>6.5551472566388897E-3</v>
+        <v>5.274003385786429E-3</v>
       </c>
       <c r="F46">
-        <v>0.82692661845389037</v>
+        <v>0.46955139287930042</v>
       </c>
       <c r="G46">
-        <v>0.73263737175687926</v>
+        <v>0.83480001109334045</v>
       </c>
       <c r="H46">
-        <v>5.5678916895363313E-2</v>
+        <v>0.90757486346015837</v>
       </c>
       <c r="I46">
-        <v>8.5841635548835157E-2</v>
+        <v>0.31219539684782882</v>
       </c>
       <c r="J46">
-        <v>7.2366399227034861E-2</v>
+        <v>0.16892612548419861</v>
       </c>
       <c r="K46">
-        <v>5.2195014989081627E-2</v>
+        <v>6.1147837696696548E-3</v>
       </c>
       <c r="L46">
-        <v>6.3831649614973132E-2</v>
+        <v>3.375625099569092E-2</v>
       </c>
       <c r="M46">
-        <v>2.1779072963871381E-3</v>
+        <v>7.4817077918721223E-3</v>
       </c>
       <c r="N46">
-        <v>2.2917639513352461E-2</v>
+        <v>5.4018893943401404E-3</v>
       </c>
       <c r="O46">
-        <v>0.36726877792356932</v>
+        <v>0.57768263910821394</v>
       </c>
       <c r="P46">
-        <v>0.17864916720197269</v>
+        <v>0.14025502316821489</v>
       </c>
       <c r="Q46">
-        <v>6.2515056652635168E-2</v>
+        <v>7.935327201746209E-2</v>
       </c>
       <c r="R46">
-        <v>2.6695416194965831E-2</v>
+        <v>4.3508783003021613E-2</v>
       </c>
       <c r="S46">
-        <v>1.9752085439947092E-2</v>
+        <v>1.456762742781907E-2</v>
       </c>
       <c r="T46">
-        <v>1.432351835040354E-2</v>
+        <v>8.8941340366296504E-3</v>
       </c>
       <c r="U46">
-        <v>0.63738145599900498</v>
+        <v>0.66085633100902896</v>
       </c>
       <c r="V46">
-        <v>0.2408381746470219</v>
+        <v>0.21463159089297601</v>
       </c>
       <c r="W46">
-        <v>6.3796512746899889E-2</v>
+        <v>1.7539373203283099E-2</v>
       </c>
       <c r="X46">
-        <v>2.5469692865985539E-2</v>
+        <v>7.4281091526034904E-2</v>
       </c>
       <c r="Y46">
-        <v>1.457559000799603E-2</v>
+        <v>1.474569988889079E-2</v>
       </c>
       <c r="Z46">
-        <v>1.8744109400459352E-2</v>
+        <v>1.012301033191672E-3</v>
       </c>
       <c r="AA46">
-        <v>0.1014102075432755</v>
+        <v>0.12739657930233689</v>
       </c>
       <c r="AB46">
-        <v>5.8564197518584798E-2</v>
+        <v>6.8236778265022391E-2</v>
       </c>
       <c r="AC46">
-        <v>4.8053822059951581E-2</v>
+        <v>5.3770575819476238E-2</v>
       </c>
       <c r="AD46">
-        <v>2.4519183803970529E-2</v>
+        <v>2.342551983058613E-2</v>
       </c>
       <c r="AE46">
-        <v>2.39028503337579E-2</v>
+        <v>2.7674092456965618E-3</v>
       </c>
       <c r="AF46">
-        <v>0.34897630219824699</v>
+        <v>0.3458131795668517</v>
       </c>
       <c r="AG46">
-        <v>0.1774203787776007</v>
+        <v>0.1065037626602537</v>
       </c>
       <c r="AH46">
-        <v>4.6022901363954753E-2</v>
+        <v>2.4276531711530939E-2</v>
       </c>
       <c r="AI46">
-        <v>6.1847320726452888E-2</v>
+        <v>2.0619216030688631E-2</v>
       </c>
       <c r="AJ46">
-        <v>1.3368205092858821E-2</v>
+        <v>1.352460619641766E-2</v>
       </c>
       <c r="AK46">
-        <v>7.3233323388613774E-3</v>
+        <v>2.017793122889746E-2</v>
       </c>
       <c r="AL46">
-        <v>0.64564788524972194</v>
+        <v>0.6830934981814103</v>
       </c>
       <c r="AM46">
-        <v>7.52465375693607E-2</v>
+        <v>0.17420007605503829</v>
       </c>
       <c r="AN46">
-        <v>7.6093998229326457E-2</v>
+        <v>1.241437225539291E-2</v>
       </c>
       <c r="AO46">
-        <v>2.763670087520553E-2</v>
+        <v>7.0725758446066656E-2</v>
       </c>
       <c r="AP46">
-        <v>2.0686667925368689E-3</v>
+        <v>7.0860193317136251E-3</v>
       </c>
       <c r="AQ46">
-        <v>3.2698309688753698E-4</v>
+        <v>1.1895785505552431E-2</v>
       </c>
       <c r="AR46">
-        <v>0.727979418221818</v>
+        <v>0.63693508260260046</v>
       </c>
       <c r="AS46">
-        <v>13.89059080863248</v>
-      </c>
-      <c r="AT46" s="9">
+        <v>12.211819053800459</v>
+      </c>
+      <c r="AT46" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>0.158296580678461</v>
+        <v>0.14569228678046861</v>
       </c>
       <c r="B47">
-        <v>0.36186058423349921</v>
+        <v>0.16444242211683149</v>
       </c>
       <c r="C47">
-        <v>0.60747550165645925</v>
+        <v>0.46019856612543247</v>
       </c>
       <c r="D47">
-        <v>2.5892560691133668E-3</v>
+        <v>2.0657172461282388E-3</v>
       </c>
       <c r="E47">
-        <v>8.1323013603452812E-3</v>
+        <v>6.5551472566388897E-3</v>
       </c>
       <c r="F47">
-        <v>0.28108104503749759</v>
+        <v>0.82692661845389037</v>
       </c>
       <c r="G47">
-        <v>0.86592684945165543</v>
+        <v>0.73263737175687926</v>
       </c>
       <c r="H47">
-        <v>0.60431594713780878</v>
+        <v>5.5678916895363313E-2</v>
       </c>
       <c r="I47">
-        <v>0.1253862319292452</v>
+        <v>8.5841635548835157E-2</v>
       </c>
       <c r="J47">
-        <v>9.4475242815380084E-2</v>
+        <v>7.2366399227034861E-2</v>
       </c>
       <c r="K47">
-        <v>4.3263207289065816E-3</v>
+        <v>5.2195014989081627E-2</v>
       </c>
       <c r="L47">
-        <v>1.5239671673460801E-2</v>
+        <v>6.3831649614973132E-2</v>
       </c>
       <c r="M47">
-        <v>5.043196328428978E-4</v>
+        <v>2.1779072963871381E-3</v>
       </c>
       <c r="N47">
-        <v>6.8978901240275593E-3</v>
+        <v>2.2917639513352461E-2</v>
       </c>
       <c r="O47">
-        <v>0.49259162132138201</v>
+        <v>0.36726877792356932</v>
       </c>
       <c r="P47">
-        <v>0.106780733770122</v>
+        <v>0.17864916720197269</v>
       </c>
       <c r="Q47">
-        <v>3.401820617795482E-2</v>
+        <v>6.2515056652635168E-2</v>
       </c>
       <c r="R47">
-        <v>1.1701273126313579E-2</v>
+        <v>2.6695416194965831E-2</v>
       </c>
       <c r="S47">
-        <v>1.6430592857149661E-2</v>
+        <v>1.9752085439947092E-2</v>
       </c>
       <c r="T47">
-        <v>1.4053946634836919E-3</v>
+        <v>1.432351835040354E-2</v>
       </c>
       <c r="U47">
-        <v>0.57483248680748078</v>
+        <v>0.63738145599900498</v>
       </c>
       <c r="V47">
-        <v>3.8437342142420887E-2</v>
+        <v>0.2408381746470219</v>
       </c>
       <c r="W47">
-        <v>4.436635610072958E-2</v>
+        <v>6.3796512746899889E-2</v>
       </c>
       <c r="X47">
-        <v>5.8329120975719781E-2</v>
+        <v>2.5469692865985539E-2</v>
       </c>
       <c r="Y47">
-        <v>1.053328830325481E-2</v>
+        <v>1.457559000799603E-2</v>
       </c>
       <c r="Z47">
-        <v>1.6735919131785831E-2</v>
+        <v>1.8744109400459352E-2</v>
       </c>
       <c r="AA47">
-        <v>5.1908868298256999E-2</v>
+        <v>0.1014102075432755</v>
       </c>
       <c r="AB47">
-        <v>1.3880048653900801E-2</v>
+        <v>5.8564197518584798E-2</v>
       </c>
       <c r="AC47">
-        <v>5.9470488451212812E-2</v>
+        <v>4.8053822059951581E-2</v>
       </c>
       <c r="AD47">
-        <v>2.1337826655503041E-2</v>
+        <v>2.4519183803970529E-2</v>
       </c>
       <c r="AE47">
-        <v>9.4119315182983835E-3</v>
+        <v>2.39028503337579E-2</v>
       </c>
       <c r="AF47">
-        <v>0.15174977497670461</v>
+        <v>0.34897630219824699</v>
       </c>
       <c r="AG47">
-        <v>0.1725911824550922</v>
+        <v>0.1774203787776007</v>
       </c>
       <c r="AH47">
-        <v>6.8965086984520384E-3</v>
+        <v>4.6022901363954753E-2</v>
       </c>
       <c r="AI47">
-        <v>7.8842246876385857E-2</v>
+        <v>6.1847320726452888E-2</v>
       </c>
       <c r="AJ47">
-        <v>1.441657483075282E-2</v>
+        <v>1.3368205092858821E-2</v>
       </c>
       <c r="AK47">
-        <v>7.7821730881729142E-3</v>
+        <v>7.3233323388613774E-3</v>
       </c>
       <c r="AL47">
-        <v>0.55859516716333357</v>
+        <v>0.64564788524972194</v>
       </c>
       <c r="AM47">
-        <v>0.19890456736966519</v>
+        <v>7.52465375693607E-2</v>
       </c>
       <c r="AN47">
-        <v>3.9204983795086334E-3</v>
+        <v>7.6093998229326457E-2</v>
       </c>
       <c r="AO47">
-        <v>7.2982843181920803E-2</v>
+        <v>2.763670087520553E-2</v>
       </c>
       <c r="AP47">
-        <v>3.3419387709997311E-3</v>
+        <v>2.0686667925368689E-3</v>
       </c>
       <c r="AQ47">
-        <v>1.0969602167583071E-2</v>
+        <v>3.2698309688753698E-4</v>
       </c>
       <c r="AR47">
-        <v>0.8250198841939208</v>
+        <v>0.727979418221818</v>
       </c>
       <c r="AS47">
-        <v>14.809973759231751</v>
-      </c>
-      <c r="AT47" s="9">
+        <v>13.89059080863248</v>
+      </c>
+      <c r="AT47" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>5.9014416942380937E-2</v>
+        <v>0.158296580678461</v>
       </c>
       <c r="B48">
-        <v>0.48784895505912351</v>
+        <v>0.36186058423349921</v>
       </c>
       <c r="C48">
-        <v>0.28487699832750968</v>
+        <v>0.60747550165645925</v>
       </c>
       <c r="D48">
-        <v>5.697022437279764E-3</v>
+        <v>2.5892560691133668E-3</v>
       </c>
       <c r="E48">
-        <v>7.2349947714034132E-3</v>
+        <v>8.1323013603452812E-3</v>
       </c>
       <c r="F48">
-        <v>0.45849621535209317</v>
+        <v>0.28108104503749759</v>
       </c>
       <c r="G48">
-        <v>0.38518597298727719</v>
+        <v>0.86592684945165543</v>
       </c>
       <c r="H48">
-        <v>0.75919616270413015</v>
+        <v>0.60431594713780878</v>
       </c>
       <c r="I48">
-        <v>7.2059857881990319E-2</v>
+        <v>0.1253862319292452</v>
       </c>
       <c r="J48">
-        <v>9.2072372625980697E-2</v>
+        <v>9.4475242815380084E-2</v>
       </c>
       <c r="K48">
-        <v>2.692931714147186E-2</v>
+        <v>4.3263207289065816E-3</v>
       </c>
       <c r="L48">
-        <v>4.1400881964034672E-2</v>
+        <v>1.5239671673460801E-2</v>
       </c>
       <c r="M48">
-        <v>1.8787154924152949E-3</v>
+        <v>5.043196328428978E-4</v>
       </c>
       <c r="N48">
-        <v>1.378977832655353E-2</v>
+        <v>6.8978901240275593E-3</v>
       </c>
       <c r="O48">
-        <v>0.32577825644815239</v>
+        <v>0.49259162132138201</v>
       </c>
       <c r="P48">
-        <v>0.20052847645182589</v>
+        <v>0.106780733770122</v>
       </c>
       <c r="Q48">
-        <v>3.4320356903148538E-2</v>
+        <v>3.401820617795482E-2</v>
       </c>
       <c r="R48">
-        <v>5.818967336484944E-2</v>
+        <v>1.1701273126313579E-2</v>
       </c>
       <c r="S48">
-        <v>1.7053918216936311E-4</v>
+        <v>1.6430592857149661E-2</v>
       </c>
       <c r="T48">
-        <v>8.7482466766471874E-3</v>
+        <v>1.4053946634836919E-3</v>
       </c>
       <c r="U48">
-        <v>0.3468097949182064</v>
+        <v>0.57483248680748078</v>
       </c>
       <c r="V48">
-        <v>6.3755812048534755E-2</v>
+        <v>3.8437342142420887E-2</v>
       </c>
       <c r="W48">
-        <v>6.6967590724101175E-2</v>
+        <v>4.436635610072958E-2</v>
       </c>
       <c r="X48">
-        <v>8.0082318408825001E-2</v>
+        <v>5.8329120975719781E-2</v>
       </c>
       <c r="Y48">
-        <v>1.307053260078537E-2</v>
+        <v>1.053328830325481E-2</v>
       </c>
       <c r="Z48">
-        <v>2.3150741938132539E-2</v>
+        <v>1.6735919131785831E-2</v>
       </c>
       <c r="AA48">
-        <v>5.446834140352369E-2</v>
+        <v>5.1908868298256999E-2</v>
       </c>
       <c r="AB48">
-        <v>5.3268681400547711E-2</v>
+        <v>1.3880048653900801E-2</v>
       </c>
       <c r="AC48">
-        <v>7.2296799712420201E-2</v>
+        <v>5.9470488451212812E-2</v>
       </c>
       <c r="AD48">
-        <v>5.2423467128931704E-4</v>
+        <v>2.1337826655503041E-2</v>
       </c>
       <c r="AE48">
-        <v>3.2522671664910737E-4</v>
+        <v>9.4119315182983835E-3</v>
       </c>
       <c r="AF48">
-        <v>0.43444002264090048</v>
+        <v>0.15174977497670461</v>
       </c>
       <c r="AG48">
-        <v>8.5603505429521221E-3</v>
+        <v>0.1725911824550922</v>
       </c>
       <c r="AH48">
-        <v>6.0914722909721171E-2</v>
+        <v>6.8965086984520384E-3</v>
       </c>
       <c r="AI48">
-        <v>1.5389968389825089E-2</v>
+        <v>7.8842246876385857E-2</v>
       </c>
       <c r="AJ48">
-        <v>3.739418378241269E-3</v>
+        <v>1.441657483075282E-2</v>
       </c>
       <c r="AK48">
-        <v>2.427254383552158E-2</v>
+        <v>7.7821730881729142E-3</v>
       </c>
       <c r="AL48">
-        <v>0.43624594043216591</v>
+        <v>0.55859516716333357</v>
       </c>
       <c r="AM48">
-        <v>0.18737054823548821</v>
+        <v>0.19890456736966519</v>
       </c>
       <c r="AN48">
-        <v>8.3741426125603959E-3</v>
+        <v>3.9204983795086334E-3</v>
       </c>
       <c r="AO48">
-        <v>8.2378656665631447E-2</v>
+        <v>7.2982843181920803E-2</v>
       </c>
       <c r="AP48">
-        <v>1.791298051465973E-2</v>
+        <v>3.3419387709997311E-3</v>
       </c>
       <c r="AQ48">
-        <v>6.5506609317727404E-3</v>
+        <v>1.0969602167583071E-2</v>
       </c>
       <c r="AR48">
-        <v>0.97083439755605438</v>
+        <v>0.8250198841939208</v>
       </c>
       <c r="AS48">
-        <v>17.75617013975307</v>
-      </c>
-      <c r="AT48" s="9">
+        <v>14.809973759231751</v>
+      </c>
+      <c r="AT48" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>3.6244261361084988E-2</v>
+        <v>5.9014416942380937E-2</v>
       </c>
       <c r="B49">
-        <v>0.64333584103691088</v>
+        <v>0.48784895505912351</v>
       </c>
       <c r="C49">
-        <v>5.6741496087908461E-2</v>
+        <v>0.28487699832750968</v>
       </c>
       <c r="D49">
-        <v>8.076967570607994E-3</v>
+        <v>5.697022437279764E-3</v>
       </c>
       <c r="E49">
-        <v>6.9631999405458771E-3</v>
+        <v>7.2349947714034132E-3</v>
       </c>
       <c r="F49">
-        <v>0.12770112018919949</v>
+        <v>0.45849621535209317</v>
       </c>
       <c r="G49">
-        <v>2.077092723834539E-2</v>
+        <v>0.38518597298727719</v>
       </c>
       <c r="H49">
-        <v>0.69203721892643222</v>
+        <v>0.75919616270413015</v>
       </c>
       <c r="I49">
-        <v>0.13923533288323819</v>
+        <v>7.2059857881990319E-2</v>
       </c>
       <c r="J49">
-        <v>6.0112043045371683E-2</v>
+        <v>9.2072372625980697E-2</v>
       </c>
       <c r="K49">
-        <v>7.5434876110918064E-2</v>
+        <v>2.692931714147186E-2</v>
       </c>
       <c r="L49">
-        <v>6.4667379982486844E-3</v>
+        <v>4.1400881964034672E-2</v>
       </c>
       <c r="M49">
-        <v>3.7996732312156611E-4</v>
+        <v>1.8787154924152949E-3</v>
       </c>
       <c r="N49">
-        <v>1.0860069939103391E-2</v>
+        <v>1.378977832655353E-2</v>
       </c>
       <c r="O49">
-        <v>0.45100645155151481</v>
+        <v>0.32577825644815239</v>
       </c>
       <c r="P49">
-        <v>0.18665675889463951</v>
+        <v>0.20052847645182589</v>
       </c>
       <c r="Q49">
-        <v>3.9602489740293657E-2</v>
+        <v>3.4320356903148538E-2</v>
       </c>
       <c r="R49">
-        <v>3.4333730743430602E-2</v>
+        <v>5.818967336484944E-2</v>
       </c>
       <c r="S49">
-        <v>2.9109833433985629E-3</v>
+        <v>1.7053918216936311E-4</v>
       </c>
       <c r="T49">
-        <v>3.5388349435535971E-3</v>
+        <v>8.7482466766471874E-3</v>
       </c>
       <c r="U49">
-        <v>0.48234947033968562</v>
+        <v>0.3468097949182064</v>
       </c>
       <c r="V49">
-        <v>0.1194164360181916</v>
+        <v>6.3755812048534755E-2</v>
       </c>
       <c r="W49">
-        <v>1.9418666630945661E-2</v>
+        <v>6.6967590724101175E-2</v>
       </c>
       <c r="X49">
-        <v>2.368711466861614E-2</v>
+        <v>8.0082318408825001E-2</v>
       </c>
       <c r="Y49">
-        <v>2.1688904170332819E-2</v>
+        <v>1.307053260078537E-2</v>
       </c>
       <c r="Z49">
-        <v>6.6858287000949512E-3</v>
+        <v>2.3150741938132539E-2</v>
       </c>
       <c r="AA49">
-        <v>0.13509025046024389</v>
+        <v>5.446834140352369E-2</v>
       </c>
       <c r="AB49">
-        <v>5.3546250762029408E-2</v>
+        <v>5.3268681400547711E-2</v>
       </c>
       <c r="AC49">
-        <v>4.8598950888950943E-2</v>
+        <v>7.2296799712420201E-2</v>
       </c>
       <c r="AD49">
-        <v>9.9521273649075884E-3</v>
+        <v>5.2423467128931704E-4</v>
       </c>
       <c r="AE49">
-        <v>3.4769129518746312E-3</v>
+        <v>3.2522671664910737E-4</v>
       </c>
       <c r="AF49">
-        <v>0.37374676766311649</v>
+        <v>0.43444002264090048</v>
       </c>
       <c r="AG49">
-        <v>5.9383100406942863E-2</v>
+        <v>8.5603505429521221E-3</v>
       </c>
       <c r="AH49">
-        <v>3.3191581435183283E-2</v>
+        <v>6.0914722909721171E-2</v>
       </c>
       <c r="AI49">
-        <v>4.437135980879138E-2</v>
+        <v>1.5389968389825089E-2</v>
       </c>
       <c r="AJ49">
-        <v>1.8367038289865339E-2</v>
+        <v>3.739418378241269E-3</v>
       </c>
       <c r="AK49">
-        <v>4.0478788104104102E-3</v>
+        <v>2.427254383552158E-2</v>
       </c>
       <c r="AL49">
-        <v>0.1811914299616024</v>
+        <v>0.43624594043216591</v>
       </c>
       <c r="AM49">
-        <v>0.20271235448241309</v>
+        <v>0.18737054823548821</v>
       </c>
       <c r="AN49">
-        <v>2.385062617594845E-2</v>
+        <v>8.3741426125603959E-3</v>
       </c>
       <c r="AO49">
-        <v>7.8457904079325166E-2</v>
+        <v>8.2378656665631447E-2</v>
       </c>
       <c r="AP49">
-        <v>1.3798717352006269E-3</v>
+        <v>1.791298051465973E-2</v>
       </c>
       <c r="AQ49">
-        <v>2.281903572171412E-2</v>
+        <v>6.5506609317727404E-3</v>
       </c>
       <c r="AR49">
-        <v>4.4796870203235417E-2</v>
+        <v>0.97083439755605438</v>
       </c>
       <c r="AS49">
-        <v>20.526127524448231</v>
-      </c>
-      <c r="AT49" s="9">
+        <v>17.75617013975307</v>
+      </c>
+      <c r="AT49" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>3.8153129081649188E-2</v>
+        <v>3.6244261361084988E-2</v>
       </c>
       <c r="B50">
-        <v>0.92915486408930126</v>
+        <v>0.64333584103691088</v>
       </c>
       <c r="C50">
-        <v>0.12781329154081841</v>
+        <v>5.6741496087908461E-2</v>
       </c>
       <c r="D50">
-        <v>8.0062086052821307E-3</v>
+        <v>8.076967570607994E-3</v>
       </c>
       <c r="E50">
-        <v>4.8576545793028083E-3</v>
+        <v>6.9631999405458771E-3</v>
       </c>
       <c r="F50">
-        <v>0.65950638794973004</v>
+        <v>0.12770112018919949</v>
       </c>
       <c r="G50">
-        <v>9.2626622618909082E-2</v>
+        <v>2.077092723834539E-2</v>
       </c>
       <c r="H50">
-        <v>4.0094850734237457E-2</v>
+        <v>0.69203721892643222</v>
       </c>
       <c r="I50">
-        <v>0.2878380789161854</v>
+        <v>0.13923533288323819</v>
       </c>
       <c r="J50">
-        <v>5.4253171195572741E-2</v>
+        <v>6.0112043045371683E-2</v>
       </c>
       <c r="K50">
-        <v>5.2596947648911811E-2</v>
+        <v>7.5434876110918064E-2</v>
       </c>
       <c r="L50">
-        <v>4.5187728453062487E-2</v>
+        <v>6.4667379982486844E-3</v>
       </c>
       <c r="M50">
-        <v>1.520707451079783E-2</v>
+        <v>3.7996732312156611E-4</v>
       </c>
       <c r="N50">
-        <v>7.3645837161629704E-4</v>
+        <v>1.0860069939103391E-2</v>
       </c>
       <c r="O50">
-        <v>0.42487338083315551</v>
+        <v>0.45100645155151481</v>
       </c>
       <c r="P50">
-        <v>0.19417534047793081</v>
+        <v>0.18665675889463951</v>
       </c>
       <c r="Q50">
-        <v>5.8977289702792958E-2</v>
+        <v>3.9602489740293657E-2</v>
       </c>
       <c r="R50">
-        <v>5.0226173506369792E-2</v>
+        <v>3.4333730743430602E-2</v>
       </c>
       <c r="S50">
-        <v>4.7098764430435038E-3</v>
+        <v>2.9109833433985629E-3</v>
       </c>
       <c r="T50">
-        <v>1.512992886106827E-2</v>
+        <v>3.5388349435535971E-3</v>
       </c>
       <c r="U50">
-        <v>0.61004018945301974</v>
+        <v>0.48234947033968562</v>
       </c>
       <c r="V50">
-        <v>0.21354367549930159</v>
+        <v>0.1194164360181916</v>
       </c>
       <c r="W50">
-        <v>6.951437262510457E-2</v>
+        <v>1.9418666630945661E-2</v>
       </c>
       <c r="X50">
-        <v>5.8637406718124258E-2</v>
+        <v>2.368711466861614E-2</v>
       </c>
       <c r="Y50">
-        <v>9.2365324321409762E-3</v>
+        <v>2.1688904170332819E-2</v>
       </c>
       <c r="Z50">
-        <v>1.5034407013543171E-3</v>
+        <v>6.6858287000949512E-3</v>
       </c>
       <c r="AA50">
-        <v>0.19143216557696111</v>
+        <v>0.13509025046024389</v>
       </c>
       <c r="AB50">
-        <v>1.5523158270562221E-2</v>
+        <v>5.3546250762029408E-2</v>
       </c>
       <c r="AC50">
-        <v>7.5338658413116502E-2</v>
+        <v>4.8598950888950943E-2</v>
       </c>
       <c r="AD50">
-        <v>1.4897157093826359E-2</v>
+        <v>9.9521273649075884E-3</v>
       </c>
       <c r="AE50">
-        <v>4.083740184845217E-3</v>
+        <v>3.4769129518746312E-3</v>
       </c>
       <c r="AF50">
-        <v>0.2498955278477559</v>
+        <v>0.37374676766311649</v>
       </c>
       <c r="AG50">
-        <v>9.1654053879282854E-2</v>
+        <v>5.9383100406942863E-2</v>
       </c>
       <c r="AH50">
-        <v>3.2735724067990697E-2</v>
+        <v>3.3191581435183283E-2</v>
       </c>
       <c r="AI50">
-        <v>5.5384535966352913E-2</v>
+        <v>4.437135980879138E-2</v>
       </c>
       <c r="AJ50">
-        <v>4.8725109136479317E-3</v>
+        <v>1.8367038289865339E-2</v>
       </c>
       <c r="AK50">
-        <v>1.7177377527079159E-2</v>
+        <v>4.0478788104104102E-3</v>
       </c>
       <c r="AL50">
-        <v>0.55437711277372381</v>
+        <v>0.1811914299616024</v>
       </c>
       <c r="AM50">
-        <v>0.14709698499770241</v>
+        <v>0.20271235448241309</v>
       </c>
       <c r="AN50">
-        <v>9.339344126633644E-3</v>
+        <v>2.385062617594845E-2</v>
       </c>
       <c r="AO50">
-        <v>1.6800358791196731E-2</v>
+        <v>7.8457904079325166E-2</v>
       </c>
       <c r="AP50">
-        <v>2.3114608501739568E-2</v>
+        <v>1.3798717352006269E-3</v>
       </c>
       <c r="AQ50">
-        <v>1.5059269531334281E-2</v>
+        <v>2.281903572171412E-2</v>
       </c>
       <c r="AR50">
-        <v>0.3141223657729072</v>
+        <v>4.4796870203235417E-2</v>
       </c>
       <c r="AS50">
-        <v>24.021836404275831</v>
-      </c>
-      <c r="AT50" s="9">
+        <v>20.526127524448231</v>
+      </c>
+      <c r="AT50" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>4.3888599573578671E-2</v>
+        <v>0.13805431398096171</v>
       </c>
       <c r="B51">
-        <v>9.2548797019443851E-2</v>
+        <v>0.78282323788731056</v>
       </c>
       <c r="C51">
-        <v>0.32777448001466752</v>
+        <v>0.60893711699058273</v>
       </c>
       <c r="D51">
-        <v>4.9279008281274501E-3</v>
+        <v>3.4200398949385319E-3</v>
       </c>
       <c r="E51">
-        <v>1.361437117196933E-2</v>
+        <v>5.8817111413591791E-3</v>
       </c>
       <c r="F51">
-        <v>0.92369682563961097</v>
+        <v>0.8497413335610392</v>
       </c>
       <c r="G51">
-        <v>0.14238383975630389</v>
+        <v>0.33717400290936628</v>
       </c>
       <c r="H51">
-        <v>0.8225024449117212</v>
+        <v>0.65234855355033461</v>
       </c>
       <c r="I51">
-        <v>0.23494246540587399</v>
+        <v>0.1233167644160361</v>
       </c>
       <c r="J51">
-        <v>0.1063503221845338</v>
+        <v>6.6985095810262657E-2</v>
       </c>
       <c r="K51">
-        <v>7.466597393402343E-3</v>
+        <v>1.9010469911640421E-2</v>
       </c>
       <c r="L51">
-        <v>6.2024020541554307E-2</v>
+        <v>5.87733131339142E-2</v>
       </c>
       <c r="M51">
-        <v>1.23402652355295E-2</v>
+        <v>2.0010496302112421E-2</v>
       </c>
       <c r="N51">
-        <v>6.7984627885338718E-3</v>
+        <v>7.700775174732658E-3</v>
       </c>
       <c r="O51">
-        <v>0.48332919750391762</v>
+        <v>0.63322451887438502</v>
       </c>
       <c r="P51">
-        <v>3.4788724925084169E-3</v>
+        <v>0.15380783257624939</v>
       </c>
       <c r="Q51">
-        <v>7.6530744931397443E-2</v>
+        <v>4.9537222504913207E-2</v>
       </c>
       <c r="R51">
-        <v>5.5557785186409643E-2</v>
+        <v>2.3647502428010198E-3</v>
       </c>
       <c r="S51">
-        <v>1.053415416694478E-2</v>
+        <v>1.5244690608115161E-2</v>
       </c>
       <c r="T51">
-        <v>2.003501054877125E-2</v>
+        <v>2.0239819135348339E-2</v>
       </c>
       <c r="U51">
-        <v>0.60380888817086742</v>
+        <v>0.62875381670316854</v>
       </c>
       <c r="V51">
-        <v>0.2499462658237839</v>
+        <v>0.11885020101554621</v>
       </c>
       <c r="W51">
-        <v>6.4099686137337866E-2</v>
+        <v>3.2510362128605447E-2</v>
       </c>
       <c r="X51">
-        <v>6.0715877237914592E-2</v>
+        <v>1.086684782239917E-2</v>
       </c>
       <c r="Y51">
-        <v>2.2817879431448501E-2</v>
+        <v>9.1879034973284535E-3</v>
       </c>
       <c r="Z51">
-        <v>2.3423607383831729E-2</v>
+        <v>1.151542590115249E-2</v>
       </c>
       <c r="AA51">
-        <v>0.196982859940246</v>
+        <v>2.4220734711297431E-3</v>
       </c>
       <c r="AB51">
-        <v>3.8297763274716089E-2</v>
+        <v>7.6175212617220781E-2</v>
       </c>
       <c r="AC51">
-        <v>1.924370008476738E-2</v>
+        <v>5.4915496855090319E-2</v>
       </c>
       <c r="AD51">
-        <v>1.4071070063347331E-2</v>
+        <v>8.4238118935986983E-3</v>
       </c>
       <c r="AE51">
-        <v>2.219477671074269E-2</v>
+        <v>7.3859678392954242E-3</v>
       </c>
       <c r="AF51">
-        <v>0.33213008654213122</v>
+        <v>0.1076250256671523</v>
       </c>
       <c r="AG51">
-        <v>0.124868115930899</v>
+        <v>0.16960116411240719</v>
       </c>
       <c r="AH51">
-        <v>5.164519496386135E-2</v>
+        <v>3.1237567358794518E-4</v>
       </c>
       <c r="AI51">
-        <v>3.5631138057243723E-2</v>
+        <v>1.2581488712770461E-2</v>
       </c>
       <c r="AJ51">
-        <v>6.0537211817559807E-3</v>
+        <v>1.336627792324846E-2</v>
       </c>
       <c r="AK51">
-        <v>2.0899814533771419E-2</v>
+        <v>1.2368137920320311E-2</v>
       </c>
       <c r="AL51">
-        <v>0.27335184635105669</v>
+        <v>0.37625294819231431</v>
       </c>
       <c r="AM51">
-        <v>0.18090128207756889</v>
+        <v>0.2060284121936943</v>
       </c>
       <c r="AN51">
-        <v>4.5029201481530307E-2</v>
+        <v>4.9497869026317871E-2</v>
       </c>
       <c r="AO51">
-        <v>7.3038639810360892E-2</v>
+        <v>6.7095119933574102E-2</v>
       </c>
       <c r="AP51">
-        <v>8.4077563988226092E-3</v>
+        <v>1.268559308089918E-2</v>
       </c>
       <c r="AQ51">
-        <v>1.6954956145107891E-2</v>
+        <v>1.7990142783364589E-2</v>
       </c>
       <c r="AR51">
-        <v>0.2330619447625274</v>
+        <v>0.90805358765267286</v>
       </c>
       <c r="AS51">
-        <v>24.400221259988339</v>
-      </c>
-      <c r="AT51" s="9">
+        <v>22.9205824533712</v>
+      </c>
+      <c r="AT51" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>0.19578481000823919</v>
+        <v>3.8153129081649188E-2</v>
       </c>
       <c r="B52">
-        <v>0.50492482024759022</v>
+        <v>0.92915486408930126</v>
       </c>
       <c r="C52">
-        <v>9.7421157488413956E-2</v>
+        <v>0.12781329154081841</v>
       </c>
       <c r="D52">
-        <v>1.9619518075065282E-3</v>
+        <v>8.0062086052821307E-3</v>
       </c>
       <c r="E52">
-        <v>1.197298522286035E-2</v>
+        <v>4.8576545793028083E-3</v>
       </c>
       <c r="F52">
-        <v>0.81603298957503068</v>
+        <v>0.65950638794973004</v>
       </c>
       <c r="G52">
-        <v>0.84916377423621769</v>
+        <v>9.2626622618909082E-2</v>
       </c>
       <c r="H52">
-        <v>0.90687142516468666</v>
+        <v>4.0094850734237457E-2</v>
       </c>
       <c r="I52">
-        <v>0.37275147603447623</v>
+        <v>0.2878380789161854</v>
       </c>
       <c r="J52">
-        <v>5.3599149193923327E-2</v>
+        <v>5.4253171195572741E-2</v>
       </c>
       <c r="K52">
-        <v>7.7323845825529425E-2</v>
+        <v>5.2596947648911811E-2</v>
       </c>
       <c r="L52">
-        <v>3.6617204365853029E-2</v>
+        <v>4.5187728453062487E-2</v>
       </c>
       <c r="M52">
-        <v>9.0228104186102099E-3</v>
+        <v>1.520707451079783E-2</v>
       </c>
       <c r="N52">
-        <v>1.2400301016964649E-2</v>
+        <v>7.3645837161629704E-4</v>
       </c>
       <c r="O52">
-        <v>0.44208577328852472</v>
+        <v>0.42487338083315551</v>
       </c>
       <c r="P52">
-        <v>4.7086136173948377E-2</v>
+        <v>0.19417534047793081</v>
       </c>
       <c r="Q52">
-        <v>2.0827485773964479E-2</v>
+        <v>5.8977289702792958E-2</v>
       </c>
       <c r="R52">
-        <v>6.2392232388561897E-2</v>
+        <v>5.0226173506369792E-2</v>
       </c>
       <c r="S52">
-        <v>1.113311968029709E-2</v>
+        <v>4.7098764430435038E-3</v>
       </c>
       <c r="T52">
-        <v>5.7923079205355059E-4</v>
+        <v>1.512992886106827E-2</v>
       </c>
       <c r="U52">
-        <v>0.741883365822117</v>
+        <v>0.61004018945301974</v>
       </c>
       <c r="V52">
-        <v>8.2107683719701841E-2</v>
+        <v>0.21354367549930159</v>
       </c>
       <c r="W52">
-        <v>4.5119528562542782E-2</v>
+        <v>6.951437262510457E-2</v>
       </c>
       <c r="X52">
-        <v>2.6877909075623641E-2</v>
+        <v>5.8637406718124258E-2</v>
       </c>
       <c r="Y52">
-        <v>1.226902868315875E-2</v>
+        <v>9.2365324321409762E-3</v>
       </c>
       <c r="Z52">
-        <v>1.483126971917165E-3</v>
+        <v>1.5034407013543171E-3</v>
       </c>
       <c r="AA52">
-        <v>0.1276477181772086</v>
+        <v>0.19143216557696111</v>
       </c>
       <c r="AB52">
-        <v>3.8858346257544807E-2</v>
+        <v>1.5523158270562221E-2</v>
       </c>
       <c r="AC52">
-        <v>1.1155761600258019E-3</v>
+        <v>7.5338658413116502E-2</v>
       </c>
       <c r="AD52">
-        <v>3.514605029881638E-3</v>
+        <v>1.4897157093826359E-2</v>
       </c>
       <c r="AE52">
-        <v>1.7699545115025351E-2</v>
+        <v>4.083740184845217E-3</v>
       </c>
       <c r="AF52">
-        <v>0.36866897811106469</v>
+        <v>0.2498955278477559</v>
       </c>
       <c r="AG52">
-        <v>0.19716216002909001</v>
+        <v>9.1654053879282854E-2</v>
       </c>
       <c r="AH52">
-        <v>7.5438828603783981E-2</v>
+        <v>3.2735724067990697E-2</v>
       </c>
       <c r="AI52">
-        <v>2.210654339616052E-2</v>
+        <v>5.5384535966352913E-2</v>
       </c>
       <c r="AJ52">
-        <v>1.9755723117419771E-2</v>
+        <v>4.8725109136479317E-3</v>
       </c>
       <c r="AK52">
-        <v>1.0268552270653779E-2</v>
+        <v>1.7177377527079159E-2</v>
       </c>
       <c r="AL52">
-        <v>0.12525252686863239</v>
+        <v>0.55437711277372381</v>
       </c>
       <c r="AM52">
-        <v>2.329507710897746E-2</v>
+        <v>0.14709698499770241</v>
       </c>
       <c r="AN52">
-        <v>6.3072579429630099E-2</v>
+        <v>9.339344126633644E-3</v>
       </c>
       <c r="AO52">
-        <v>6.6254577103681947E-2</v>
+        <v>1.6800358791196731E-2</v>
       </c>
       <c r="AP52">
-        <v>2.1076892718937531E-2</v>
+        <v>2.3114608501739568E-2</v>
       </c>
       <c r="AQ52">
-        <v>2.03862181317697E-2</v>
+        <v>1.5059269531334281E-2</v>
       </c>
       <c r="AR52">
-        <v>0.34505201379039457</v>
+        <v>0.3141223657729072</v>
       </c>
       <c r="AS52">
-        <v>42.381378868530398</v>
-      </c>
-      <c r="AT52" s="9">
+        <v>24.021836404275831</v>
+      </c>
+      <c r="AT52" s="2">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="AU52" s="1"/>
     </row>
     <row r="53" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>9.582330671642561E-2</v>
+        <v>4.3888599573578671E-2</v>
       </c>
       <c r="B53">
-        <v>0.81876768576788017</v>
+        <v>9.2548797019443851E-2</v>
       </c>
       <c r="C53">
-        <v>0.59275043337493516</v>
+        <v>0.32777448001466752</v>
       </c>
       <c r="D53">
-        <v>5.8256832192755143E-3</v>
+        <v>4.9279008281274501E-3</v>
       </c>
       <c r="E53">
-        <v>1.8473385523778949E-2</v>
+        <v>1.361437117196933E-2</v>
       </c>
       <c r="F53">
-        <v>0.4825994854156882</v>
+        <v>0.92369682563961097</v>
       </c>
       <c r="G53">
-        <v>0.17305097790861321</v>
+        <v>0.14238383975630389</v>
       </c>
       <c r="H53">
-        <v>0.68350539694373358</v>
+        <v>0.8225024449117212</v>
       </c>
       <c r="I53">
-        <v>0.58044976638038404</v>
+        <v>0.23494246540587399</v>
       </c>
       <c r="J53">
-        <v>2.0010395366396479E-2</v>
+        <v>0.1063503221845338</v>
       </c>
       <c r="K53">
-        <v>6.6444184792463265E-2</v>
+        <v>7.466597393402343E-3</v>
       </c>
       <c r="L53">
-        <v>2.6015637328077701E-3</v>
+        <v>6.2024020541554307E-2</v>
       </c>
       <c r="M53">
-        <v>1.0107217286014211E-2</v>
+        <v>1.23402652355295E-2</v>
       </c>
       <c r="N53">
-        <v>8.4765420628827391E-3</v>
+        <v>6.7984627885338718E-3</v>
       </c>
       <c r="O53">
-        <v>0.40231236690815309</v>
+        <v>0.48332919750391762</v>
       </c>
       <c r="P53">
-        <v>0.1083975656618964</v>
+        <v>3.4788724925084169E-3</v>
       </c>
       <c r="Q53">
-        <v>3.7407352986408703E-2</v>
+        <v>7.6530744931397443E-2</v>
       </c>
       <c r="R53">
-        <v>6.459240174126922E-2</v>
+        <v>5.5557785186409643E-2</v>
       </c>
       <c r="S53">
-        <v>1.996480205453522E-2</v>
+        <v>1.053415416694478E-2</v>
       </c>
       <c r="T53">
-        <v>1.817898881477184E-2</v>
+        <v>2.003501054877125E-2</v>
       </c>
       <c r="U53">
-        <v>0.34176438736555848</v>
+        <v>0.60380888817086742</v>
       </c>
       <c r="V53">
-        <v>0.11711767789441881</v>
+        <v>0.2499462658237839</v>
       </c>
       <c r="W53">
-        <v>3.7812672868666172E-2</v>
+        <v>6.4099686137337866E-2</v>
       </c>
       <c r="X53">
-        <v>7.4776749679092133E-2</v>
+        <v>6.0715877237914592E-2</v>
       </c>
       <c r="Y53">
-        <v>1.953663430391164E-2</v>
+        <v>2.2817879431448501E-2</v>
       </c>
       <c r="Z53">
-        <v>1.3868114337065409E-2</v>
+        <v>2.3423607383831729E-2</v>
       </c>
       <c r="AA53">
-        <v>0.192648241554669</v>
+        <v>0.196982859940246</v>
       </c>
       <c r="AB53">
-        <v>7.7902306934244589E-3</v>
+        <v>3.8297763274716089E-2</v>
       </c>
       <c r="AC53">
-        <v>7.9640080425083817E-2</v>
+        <v>1.924370008476738E-2</v>
       </c>
       <c r="AD53">
-        <v>8.2652014062155107E-3</v>
+        <v>1.4071070063347331E-2</v>
       </c>
       <c r="AE53">
-        <v>3.2890565613926449E-3</v>
+        <v>2.219477671074269E-2</v>
       </c>
       <c r="AF53">
-        <v>0.43041308986751958</v>
+        <v>0.33213008654213122</v>
       </c>
       <c r="AG53">
-        <v>7.6834455476513797E-3</v>
+        <v>0.124868115930899</v>
       </c>
       <c r="AH53">
-        <v>7.8951310678613218E-2</v>
+        <v>5.164519496386135E-2</v>
       </c>
       <c r="AI53">
-        <v>8.0736867770604029E-2</v>
+        <v>3.5631138057243723E-2</v>
       </c>
       <c r="AJ53">
-        <v>2.1386111005674221E-2</v>
+        <v>6.0537211817559807E-3</v>
       </c>
       <c r="AK53">
-        <v>4.1637393191566513E-3</v>
+        <v>2.0899814533771419E-2</v>
       </c>
       <c r="AL53">
-        <v>3.581729121851665E-2</v>
+        <v>0.27335184635105669</v>
       </c>
       <c r="AM53">
-        <v>0.1430971270030463</v>
+        <v>0.18090128207756889</v>
       </c>
       <c r="AN53">
-        <v>3.3833842922891967E-2</v>
+        <v>4.5029201481530307E-2</v>
       </c>
       <c r="AO53">
-        <v>3.1272351657313631E-2</v>
+        <v>7.3038639810360892E-2</v>
       </c>
       <c r="AP53">
-        <v>2.0734939857887789E-2</v>
+        <v>8.4077563988226092E-3</v>
       </c>
       <c r="AQ53">
-        <v>3.5003280414894651E-3</v>
+        <v>1.6954956145107891E-2</v>
       </c>
       <c r="AR53">
-        <v>0.80147662686885901</v>
+        <v>0.2330619447625274</v>
       </c>
       <c r="AS53">
-        <v>43.507946258853643</v>
-      </c>
-      <c r="AT53" s="9">
+        <v>24.400221259988339</v>
+      </c>
+      <c r="AT53" s="2">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>0.18091972288411329</v>
+        <v>0.1070449877421773</v>
       </c>
       <c r="B54">
-        <v>0.96621326931256157</v>
+        <v>0.29154123292341549</v>
       </c>
       <c r="C54">
-        <v>0.60954520322483952</v>
+        <v>6.6333967739365951E-2</v>
       </c>
       <c r="D54">
-        <v>5.0252372589467869E-3</v>
+        <v>2.5478886876918851E-3</v>
       </c>
       <c r="E54">
-        <v>5.5450127616360166E-3</v>
+        <v>2.4639355020977601E-3</v>
       </c>
       <c r="F54">
-        <v>0.65805756020959671</v>
+        <v>1.520658827236987E-2</v>
       </c>
       <c r="G54">
-        <v>0.32882694906799442</v>
+        <v>0.52612380855732632</v>
       </c>
       <c r="H54">
-        <v>0.6235270275086795</v>
+        <v>0.79320903567144407</v>
       </c>
       <c r="I54">
-        <v>0.58999572028401126</v>
+        <v>0.53932507750399339</v>
       </c>
       <c r="J54">
-        <v>2.1103412521579989E-2</v>
+        <v>7.3174477289483952E-2</v>
       </c>
       <c r="K54">
-        <v>1.2261338266301779E-2</v>
+        <v>4.4753288892984348E-2</v>
       </c>
       <c r="L54">
-        <v>2.1239475623638301E-2</v>
+        <v>6.6239697247030938E-2</v>
       </c>
       <c r="M54">
-        <v>2.024330022008477E-3</v>
+        <v>2.3046178644155171E-2</v>
       </c>
       <c r="N54">
-        <v>1.8955521913963481E-2</v>
+        <v>1.424704315522244E-2</v>
       </c>
       <c r="O54">
-        <v>0.59819261305811744</v>
+        <v>0.52385964102602389</v>
       </c>
       <c r="P54">
-        <v>0.17483634758110239</v>
+        <v>2.5555248967710831E-2</v>
       </c>
       <c r="Q54">
-        <v>2.4061863838083539E-2</v>
+        <v>8.1680279382241955E-2</v>
       </c>
       <c r="R54">
-        <v>3.3619307350697403E-2</v>
+        <v>5.1856202404127853E-2</v>
       </c>
       <c r="S54">
-        <v>2.2756019676607762E-2</v>
+        <v>8.3267811347564318E-3</v>
       </c>
       <c r="T54">
-        <v>2.3599547705056959E-2</v>
+        <v>2.1147669803558582E-2</v>
       </c>
       <c r="U54">
-        <v>0.59547076730875592</v>
+        <v>0.39837682745739272</v>
       </c>
       <c r="V54">
-        <v>1.224634273591574E-2</v>
+        <v>0.2240148055307008</v>
       </c>
       <c r="W54">
-        <v>5.2233958297657713E-3</v>
+        <v>5.1301724994894618E-2</v>
       </c>
       <c r="X54">
-        <v>6.8609428706958547E-2</v>
+        <v>3.4544709071076152E-2</v>
       </c>
       <c r="Y54">
-        <v>1.7053086438815401E-3</v>
+        <v>1.2148135456882611E-2</v>
       </c>
       <c r="Z54">
-        <v>1.3827415056087141E-4</v>
+        <v>5.2992238720002589E-3</v>
       </c>
       <c r="AA54">
-        <v>0.16203335960648271</v>
+        <v>0.2298388768072453</v>
       </c>
       <c r="AB54">
-        <v>7.7598025534525938E-2</v>
+        <v>3.6657903176635392E-2</v>
       </c>
       <c r="AC54">
-        <v>5.7019177895312328E-2</v>
+        <v>1.3791356876947349E-2</v>
       </c>
       <c r="AD54">
-        <v>4.8454554429255142E-3</v>
+        <v>1.4488718341485719E-2</v>
       </c>
       <c r="AE54">
-        <v>6.9910223849601882E-3</v>
+        <v>4.3805422778052799E-3</v>
       </c>
       <c r="AF54">
-        <v>0.47282403435022868</v>
+        <v>0.44082596013878922</v>
       </c>
       <c r="AG54">
-        <v>0.14393403619677211</v>
+        <v>0.19108860760199189</v>
       </c>
       <c r="AH54">
-        <v>4.0140748360101383E-2</v>
+        <v>3.1956701316534442E-2</v>
       </c>
       <c r="AI54">
-        <v>1.6736887854452671E-2</v>
+        <v>4.1134421217829523E-2</v>
       </c>
       <c r="AJ54">
-        <v>1.073987245280539E-2</v>
+        <v>1.218744530970175E-2</v>
       </c>
       <c r="AK54">
-        <v>1.6892252114992231E-2</v>
+        <v>3.6527914369414988E-4</v>
       </c>
       <c r="AL54">
-        <v>0.2573710078185264</v>
+        <v>0.38648929608920862</v>
       </c>
       <c r="AM54">
-        <v>0.1240047159613361</v>
+        <v>0.1202433324684905</v>
       </c>
       <c r="AN54">
-        <v>4.3186953806671237E-2</v>
+        <v>4.8564095829544837E-2</v>
       </c>
       <c r="AO54">
-        <v>8.0751133760633795E-2</v>
+        <v>1.63785664915275E-2</v>
       </c>
       <c r="AP54">
-        <v>7.6821403633477812E-3</v>
+        <v>8.0316511694180619E-3</v>
       </c>
       <c r="AQ54">
-        <v>2.2147959112184309E-2</v>
+        <v>4.1866663283612552E-3</v>
       </c>
       <c r="AR54">
-        <v>0.6664021975993526</v>
+        <v>0.73238348824898791</v>
       </c>
       <c r="AS54">
-        <v>47.569670574336783</v>
-      </c>
-      <c r="AT54" s="9">
+        <v>30.512326457271001</v>
+      </c>
+      <c r="AT54" s="2">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="AU54" s="1"/>
     </row>
     <row r="55" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>6.0665085926573631E-2</v>
+        <v>0.19578481000823919</v>
       </c>
       <c r="B55">
-        <v>0.47272629839424268</v>
+        <v>0.50492482024759022</v>
       </c>
       <c r="C55">
-        <v>0.55233849554789594</v>
+        <v>9.7421157488413956E-2</v>
       </c>
       <c r="D55">
-        <v>3.2167713448302241E-3</v>
+        <v>1.9619518075065282E-3</v>
       </c>
       <c r="E55">
-        <v>6.7518868747691533E-3</v>
+        <v>1.197298522286035E-2</v>
       </c>
       <c r="F55">
-        <v>3.2038273930865217E-2</v>
+        <v>0.81603298957503068</v>
       </c>
       <c r="G55">
-        <v>0.7443096289250738</v>
+        <v>0.84916377423621769</v>
       </c>
       <c r="H55">
-        <v>3.3683522886886919E-2</v>
+        <v>0.90687142516468666</v>
       </c>
       <c r="I55">
-        <v>0.60436326203495694</v>
+        <v>0.37275147603447623</v>
       </c>
       <c r="J55">
-        <v>4.6327698980049743E-2</v>
+        <v>5.3599149193923327E-2</v>
       </c>
       <c r="K55">
-        <v>2.080651039608393E-2</v>
+        <v>7.7323845825529425E-2</v>
       </c>
       <c r="L55">
-        <v>3.2312745700035332E-2</v>
+        <v>3.6617204365853029E-2</v>
       </c>
       <c r="M55">
-        <v>1.8887187521105318E-2</v>
+        <v>9.0228104186102099E-3</v>
       </c>
       <c r="N55">
-        <v>8.7909160222302673E-3</v>
+        <v>1.2400301016964649E-2</v>
       </c>
       <c r="O55">
-        <v>0.54553465354961694</v>
+        <v>0.44208577328852472</v>
       </c>
       <c r="P55">
-        <v>4.1010297960852843E-2</v>
+        <v>4.7086136173948377E-2</v>
       </c>
       <c r="Q55">
-        <v>4.8177347438859423E-2</v>
+        <v>2.0827485773964479E-2</v>
       </c>
       <c r="R55">
-        <v>3.2153765943582692E-2</v>
+        <v>6.2392232388561897E-2</v>
       </c>
       <c r="S55">
-        <v>1.465291220286746E-3</v>
+        <v>1.113311968029709E-2</v>
       </c>
       <c r="T55">
-        <v>1.6841919612880001E-2</v>
+        <v>5.7923079205355059E-4</v>
       </c>
       <c r="U55">
-        <v>0.33200572852343918</v>
+        <v>0.741883365822117</v>
       </c>
       <c r="V55">
-        <v>3.7069671081555761E-2</v>
+        <v>8.2107683719701841E-2</v>
       </c>
       <c r="W55">
-        <v>7.1133894923729374E-2</v>
+        <v>4.5119528562542782E-2</v>
       </c>
       <c r="X55">
-        <v>4.0451876817633589E-3</v>
+        <v>2.6877909075623641E-2</v>
       </c>
       <c r="Y55">
-        <v>1.3523711440632251E-3</v>
+        <v>1.226902868315875E-2</v>
       </c>
       <c r="Z55">
-        <v>1.355887382815784E-2</v>
+        <v>1.483126971917165E-3</v>
       </c>
       <c r="AA55">
-        <v>3.2752540723000378E-2</v>
+        <v>0.1276477181772086</v>
       </c>
       <c r="AB55">
-        <v>7.8078638621362162E-2</v>
+        <v>3.8858346257544807E-2</v>
       </c>
       <c r="AC55">
-        <v>5.7632973504134273E-2</v>
+        <v>1.1155761600258019E-3</v>
       </c>
       <c r="AD55">
-        <v>5.7980528530883341E-3</v>
+        <v>3.514605029881638E-3</v>
       </c>
       <c r="AE55">
-        <v>5.6674181546491342E-4</v>
+        <v>1.7699545115025351E-2</v>
       </c>
       <c r="AF55">
-        <v>0.43839579580866328</v>
+        <v>0.36866897811106469</v>
       </c>
       <c r="AG55">
-        <v>7.8144553172492304E-2</v>
+        <v>0.19716216002909001</v>
       </c>
       <c r="AH55">
-        <v>2.40672268807102E-2</v>
+        <v>7.5438828603783981E-2</v>
       </c>
       <c r="AI55">
-        <v>3.7801840931906049E-2</v>
+        <v>2.210654339616052E-2</v>
       </c>
       <c r="AJ55">
-        <v>1.3676415548283411E-2</v>
+        <v>1.9755723117419771E-2</v>
       </c>
       <c r="AK55">
-        <v>3.5929406215859661E-3</v>
+        <v>1.0268552270653779E-2</v>
       </c>
       <c r="AL55">
-        <v>9.0318204968601407E-2</v>
+        <v>0.12525252686863239</v>
       </c>
       <c r="AM55">
-        <v>6.902522065626171E-2</v>
+        <v>2.329507710897746E-2</v>
       </c>
       <c r="AN55">
-        <v>1.237031947023043E-2</v>
+        <v>6.3072579429630099E-2</v>
       </c>
       <c r="AO55">
-        <v>9.774176640690949E-3</v>
+        <v>6.6254577103681947E-2</v>
       </c>
       <c r="AP55">
-        <v>1.1623803599190781E-2</v>
+        <v>2.1076892718937531E-2</v>
       </c>
       <c r="AQ55">
-        <v>2.03861121172998E-2</v>
+        <v>2.03862181317697E-2</v>
       </c>
       <c r="AR55">
-        <v>0.96027356293895683</v>
+        <v>0.34505201379039457</v>
       </c>
       <c r="AS55">
-        <v>47.731715945093292</v>
-      </c>
-      <c r="AT55" s="9">
+        <v>42.381378868530398</v>
+      </c>
+      <c r="AT55" s="2">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
@@ -8531,1202 +8530,1107 @@
     </row>
     <row r="56" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>0.16219245526942669</v>
+        <v>0.1261499834597638</v>
       </c>
       <c r="B56">
-        <v>0.12941459784162099</v>
+        <v>0.65491129823672156</v>
       </c>
       <c r="C56">
-        <v>1.3343855281409359E-2</v>
+        <v>3.6799802033325668E-2</v>
       </c>
       <c r="D56">
-        <v>3.1629275531599131E-3</v>
+        <v>6.6456966824786062E-3</v>
       </c>
       <c r="E56">
-        <v>5.244943294882674E-3</v>
+        <v>1.0312187571759069E-2</v>
       </c>
       <c r="F56">
-        <v>0.70103564271928542</v>
+        <v>0.92901590506206277</v>
       </c>
       <c r="G56">
-        <v>8.2541560688676463E-2</v>
+        <v>0.68967068097918571</v>
       </c>
       <c r="H56">
-        <v>0.18603477814362859</v>
+        <v>0.21142827874952691</v>
       </c>
       <c r="I56">
-        <v>0.74644441533891881</v>
+        <v>0.43306431919732291</v>
       </c>
       <c r="J56">
-        <v>0.1681442150880475</v>
+        <v>0.1173911837737634</v>
       </c>
       <c r="K56">
-        <v>7.9680780882232197E-2</v>
+        <v>2.9953591015496071E-2</v>
       </c>
       <c r="L56">
-        <v>6.5521578359597266E-2</v>
+        <v>7.7982529037466788E-2</v>
       </c>
       <c r="M56">
-        <v>1.7510693221554699E-2</v>
+        <v>2.1696856450039381E-2</v>
       </c>
       <c r="N56">
-        <v>6.4372324876934648E-3</v>
+        <v>2.1784154800143169E-3</v>
       </c>
       <c r="O56">
-        <v>0.66403841711380063</v>
+        <v>0.48806318131545828</v>
       </c>
       <c r="P56">
-        <v>2.2560098234820442E-2</v>
+        <v>7.6190045333131812E-2</v>
       </c>
       <c r="Q56">
-        <v>2.7254523550371453E-4</v>
+        <v>5.8509051641450878E-2</v>
       </c>
       <c r="R56">
-        <v>1.9965140814615041E-2</v>
+        <v>4.8957467091291576E-3</v>
       </c>
       <c r="S56">
-        <v>3.1442071154139388E-4</v>
+        <v>3.6955612421950231E-3</v>
       </c>
       <c r="T56">
-        <v>1.828101837393686E-2</v>
+        <v>4.2829245012443746E-3</v>
       </c>
       <c r="U56">
-        <v>0.68816218013119745</v>
+        <v>0.42635330232286672</v>
       </c>
       <c r="V56">
-        <v>0.14354382843533101</v>
+        <v>3.3721125697972497E-2</v>
       </c>
       <c r="W56">
-        <v>5.3556372887725121E-2</v>
+        <v>3.8244220362216912E-2</v>
       </c>
       <c r="X56">
-        <v>7.0321952047990688E-2</v>
+        <v>4.7087481356536849E-2</v>
       </c>
       <c r="Y56">
-        <v>1.342561567139069E-2</v>
+        <v>5.8072535075656328E-3</v>
       </c>
       <c r="Z56">
-        <v>2.3206569587973989E-2</v>
+        <v>8.6080404983483374E-3</v>
       </c>
       <c r="AA56">
-        <v>0.12078908181183021</v>
+        <v>0.16555949775161169</v>
       </c>
       <c r="AB56">
-        <v>1.2986306919215731E-2</v>
+        <v>6.2386070453491108E-2</v>
       </c>
       <c r="AC56">
-        <v>5.8429065492033611E-2</v>
+        <v>3.4475276975941369E-2</v>
       </c>
       <c r="AD56">
-        <v>2.2182626656987409E-2</v>
+        <v>8.3039526094350893E-4</v>
       </c>
       <c r="AE56">
-        <v>1.352196059903348E-2</v>
+        <v>1.1390514003541611E-2</v>
       </c>
       <c r="AF56">
-        <v>0.26901900679638058</v>
+        <v>0.1495633828430695</v>
       </c>
       <c r="AG56">
-        <v>0.1044713079838686</v>
+        <v>9.4504828316947259E-2</v>
       </c>
       <c r="AH56">
-        <v>5.3261442019813442E-2</v>
+        <v>6.1643544570611372E-2</v>
       </c>
       <c r="AI56">
-        <v>4.7401938990117971E-2</v>
+        <v>3.6268985385334407E-2</v>
       </c>
       <c r="AJ56">
-        <v>1.265966685698915E-2</v>
+        <v>2.2914974779453721E-2</v>
       </c>
       <c r="AK56">
-        <v>5.5946829778609989E-3</v>
+        <v>6.9267141387745956E-3</v>
       </c>
       <c r="AL56">
-        <v>0.25295898572824582</v>
+        <v>0.27061046435311442</v>
       </c>
       <c r="AM56">
-        <v>0.12906165303595071</v>
+        <v>0.17125381491731501</v>
       </c>
       <c r="AN56">
-        <v>1.0519419980512611E-2</v>
+        <v>6.0481863757984471E-2</v>
       </c>
       <c r="AO56">
-        <v>6.1292273475295901E-2</v>
+        <v>7.0667222522684009E-2</v>
       </c>
       <c r="AP56">
-        <v>2.4267638488172762E-3</v>
+        <v>4.2764994812932451E-4</v>
       </c>
       <c r="AQ56">
-        <v>3.4664326996320378E-3</v>
+        <v>2.136269683821725E-2</v>
       </c>
       <c r="AR56">
-        <v>0.7504843615751553</v>
+        <v>0.24974978010817081</v>
       </c>
       <c r="AS56">
-        <v>51.681438005353641</v>
-      </c>
-      <c r="AT56" s="9">
+        <v>44.191855708844038</v>
+      </c>
+      <c r="AT56" s="2">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>0.1261499834597638</v>
+        <v>0.17877049458235161</v>
       </c>
       <c r="B57">
-        <v>0.65491129823672156</v>
+        <v>0.6133644174327233</v>
       </c>
       <c r="C57">
-        <v>3.6799802033325668E-2</v>
+        <v>0.19186906865394299</v>
       </c>
       <c r="D57">
-        <v>6.6456966824786062E-3</v>
+        <v>2.8186713031514558E-3</v>
       </c>
       <c r="E57">
-        <v>1.0312187571759069E-2</v>
+        <v>2.1802113281694381E-2</v>
       </c>
       <c r="F57">
-        <v>0.92901590506206277</v>
+        <v>0.29862934725895268</v>
       </c>
       <c r="G57">
-        <v>0.68967068097918571</v>
+        <v>0.52083594338879247</v>
       </c>
       <c r="H57">
-        <v>0.21142827874952691</v>
+        <v>0.58741646709852691</v>
       </c>
       <c r="I57">
-        <v>0.43306431919732291</v>
+        <v>0.39444712057872477</v>
       </c>
       <c r="J57">
-        <v>0.1173911837737634</v>
+        <v>8.3700918883575476E-2</v>
       </c>
       <c r="K57">
-        <v>2.9953591015496071E-2</v>
+        <v>6.085202390806646E-2</v>
       </c>
       <c r="L57">
-        <v>7.7982529037466788E-2</v>
+        <v>2.1705301877836228E-3</v>
       </c>
       <c r="M57">
-        <v>2.1696856450039381E-2</v>
+        <v>1.814155694593156E-3</v>
       </c>
       <c r="N57">
-        <v>2.1784154800143169E-3</v>
+        <v>1.2775934700629059E-2</v>
       </c>
       <c r="O57">
-        <v>0.48806318131545828</v>
+        <v>0.555279684176198</v>
       </c>
       <c r="P57">
-        <v>7.6190045333131812E-2</v>
+        <v>0.18977823873648211</v>
       </c>
       <c r="Q57">
-        <v>5.8509051641450878E-2</v>
+        <v>1.2273604518983981E-3</v>
       </c>
       <c r="R57">
-        <v>4.8957467091291576E-3</v>
+        <v>2.5703759718509071E-2</v>
       </c>
       <c r="S57">
-        <v>3.6955612421950231E-3</v>
+        <v>1.212305287422967E-2</v>
       </c>
       <c r="T57">
-        <v>4.2829245012443746E-3</v>
+        <v>2.2305997671923421E-2</v>
       </c>
       <c r="U57">
-        <v>0.42635330232286672</v>
+        <v>0.44852038554530871</v>
       </c>
       <c r="V57">
-        <v>3.3721125697972497E-2</v>
+        <v>0.16859608908675641</v>
       </c>
       <c r="W57">
-        <v>3.8244220362216912E-2</v>
+        <v>2.7956909580341131E-2</v>
       </c>
       <c r="X57">
-        <v>4.7087481356536849E-2</v>
+        <v>2.4513958111513942E-3</v>
       </c>
       <c r="Y57">
-        <v>5.8072535075656328E-3</v>
+        <v>9.3890470115705095E-3</v>
       </c>
       <c r="Z57">
-        <v>8.6080404983483374E-3</v>
+        <v>1.0569079394492169E-3</v>
       </c>
       <c r="AA57">
-        <v>0.16555949775161169</v>
+        <v>0.11248993779002479</v>
       </c>
       <c r="AB57">
-        <v>6.2386070453491108E-2</v>
+        <v>1.27995503204822E-2</v>
       </c>
       <c r="AC57">
-        <v>3.4475276975941369E-2</v>
+        <v>4.5382720162878983E-2</v>
       </c>
       <c r="AD57">
-        <v>8.3039526094350893E-4</v>
+        <v>6.5637424036708754E-3</v>
       </c>
       <c r="AE57">
-        <v>1.1390514003541611E-2</v>
+        <v>1.7947201810540579E-2</v>
       </c>
       <c r="AF57">
-        <v>0.1495633828430695</v>
+        <v>0.31214559737667991</v>
       </c>
       <c r="AG57">
-        <v>9.4504828316947259E-2</v>
+        <v>0.13793494192439679</v>
       </c>
       <c r="AH57">
-        <v>6.1643544570611372E-2</v>
+        <v>3.6577804546072449E-3</v>
       </c>
       <c r="AI57">
-        <v>3.6268985385334407E-2</v>
+        <v>1.0494979762065079E-2</v>
       </c>
       <c r="AJ57">
-        <v>2.2914974779453721E-2</v>
+        <v>1.8290146349311271E-2</v>
       </c>
       <c r="AK57">
-        <v>6.9267141387745956E-3</v>
+        <v>2.1046084198721639E-2</v>
       </c>
       <c r="AL57">
-        <v>0.27061046435311442</v>
+        <v>0.34985261397006318</v>
       </c>
       <c r="AM57">
-        <v>0.17125381491731501</v>
+        <v>0.14239724557561409</v>
       </c>
       <c r="AN57">
-        <v>6.0481863757984471E-2</v>
+        <v>7.0690883847908392E-2</v>
       </c>
       <c r="AO57">
-        <v>7.0667222522684009E-2</v>
+        <v>7.4891355274441684E-2</v>
       </c>
       <c r="AP57">
-        <v>4.2764994812932451E-4</v>
+        <v>1.415018132722427E-2</v>
       </c>
       <c r="AQ57">
-        <v>2.136269683821725E-2</v>
+        <v>8.0473920143672999E-4</v>
       </c>
       <c r="AR57">
-        <v>0.24974978010817081</v>
+        <v>0.30370617476714901</v>
       </c>
       <c r="AS57">
-        <v>44.191855708844038</v>
-      </c>
-      <c r="AT57" s="9">
+        <v>44.301270957379693</v>
+      </c>
+      <c r="AT57" s="2">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>0.1070449877421773</v>
+        <v>0.18091972288411329</v>
       </c>
       <c r="B58">
-        <v>0.29154123292341549</v>
+        <v>0.96621326931256157</v>
       </c>
       <c r="C58">
-        <v>6.6333967739365951E-2</v>
+        <v>0.60954520322483952</v>
       </c>
       <c r="D58">
-        <v>2.5478886876918851E-3</v>
+        <v>5.0252372589467869E-3</v>
       </c>
       <c r="E58">
-        <v>2.4639355020977601E-3</v>
+        <v>5.5450127616360166E-3</v>
       </c>
       <c r="F58">
-        <v>1.520658827236987E-2</v>
+        <v>0.65805756020959671</v>
       </c>
       <c r="G58">
-        <v>0.52612380855732632</v>
+        <v>0.32882694906799442</v>
       </c>
       <c r="H58">
-        <v>0.79320903567144407</v>
+        <v>0.6235270275086795</v>
       </c>
       <c r="I58">
-        <v>0.53932507750399339</v>
+        <v>0.58999572028401126</v>
       </c>
       <c r="J58">
-        <v>7.3174477289483952E-2</v>
+        <v>2.1103412521579989E-2</v>
       </c>
       <c r="K58">
-        <v>4.4753288892984348E-2</v>
+        <v>1.2261338266301779E-2</v>
       </c>
       <c r="L58">
-        <v>6.6239697247030938E-2</v>
+        <v>2.1239475623638301E-2</v>
       </c>
       <c r="M58">
-        <v>2.3046178644155171E-2</v>
+        <v>2.024330022008477E-3</v>
       </c>
       <c r="N58">
-        <v>1.424704315522244E-2</v>
+        <v>1.8955521913963481E-2</v>
       </c>
       <c r="O58">
-        <v>0.52385964102602389</v>
+        <v>0.59819261305811744</v>
       </c>
       <c r="P58">
-        <v>2.5555248967710831E-2</v>
+        <v>0.17483634758110239</v>
       </c>
       <c r="Q58">
-        <v>8.1680279382241955E-2</v>
+        <v>2.4061863838083539E-2</v>
       </c>
       <c r="R58">
-        <v>5.1856202404127853E-2</v>
+        <v>3.3619307350697403E-2</v>
       </c>
       <c r="S58">
-        <v>8.3267811347564318E-3</v>
+        <v>2.2756019676607762E-2</v>
       </c>
       <c r="T58">
-        <v>2.1147669803558582E-2</v>
+        <v>2.3599547705056959E-2</v>
       </c>
       <c r="U58">
-        <v>0.39837682745739272</v>
+        <v>0.59547076730875592</v>
       </c>
       <c r="V58">
-        <v>0.2240148055307008</v>
+        <v>1.224634273591574E-2</v>
       </c>
       <c r="W58">
-        <v>5.1301724994894618E-2</v>
+        <v>5.2233958297657713E-3</v>
       </c>
       <c r="X58">
-        <v>3.4544709071076152E-2</v>
+        <v>6.8609428706958547E-2</v>
       </c>
       <c r="Y58">
-        <v>1.2148135456882611E-2</v>
+        <v>1.7053086438815401E-3</v>
       </c>
       <c r="Z58">
-        <v>5.2992238720002589E-3</v>
+        <v>1.3827415056087141E-4</v>
       </c>
       <c r="AA58">
-        <v>0.2298388768072453</v>
+        <v>0.16203335960648271</v>
       </c>
       <c r="AB58">
-        <v>3.6657903176635392E-2</v>
+        <v>7.7598025534525938E-2</v>
       </c>
       <c r="AC58">
-        <v>1.3791356876947349E-2</v>
+        <v>5.7019177895312328E-2</v>
       </c>
       <c r="AD58">
-        <v>1.4488718341485719E-2</v>
+        <v>4.8454554429255142E-3</v>
       </c>
       <c r="AE58">
-        <v>4.3805422778052799E-3</v>
+        <v>6.9910223849601882E-3</v>
       </c>
       <c r="AF58">
-        <v>0.44082596013878922</v>
+        <v>0.47282403435022868</v>
       </c>
       <c r="AG58">
-        <v>0.19108860760199189</v>
+        <v>0.14393403619677211</v>
       </c>
       <c r="AH58">
-        <v>3.1956701316534442E-2</v>
+        <v>4.0140748360101383E-2</v>
       </c>
       <c r="AI58">
-        <v>4.1134421217829523E-2</v>
+        <v>1.6736887854452671E-2</v>
       </c>
       <c r="AJ58">
-        <v>1.218744530970175E-2</v>
+        <v>1.073987245280539E-2</v>
       </c>
       <c r="AK58">
-        <v>3.6527914369414988E-4</v>
+        <v>1.6892252114992231E-2</v>
       </c>
       <c r="AL58">
-        <v>0.38648929608920862</v>
+        <v>0.2573710078185264</v>
       </c>
       <c r="AM58">
-        <v>0.1202433324684905</v>
+        <v>0.1240047159613361</v>
       </c>
       <c r="AN58">
-        <v>4.8564095829544837E-2</v>
+        <v>4.3186953806671237E-2</v>
       </c>
       <c r="AO58">
-        <v>1.63785664915275E-2</v>
+        <v>8.0751133760633795E-2</v>
       </c>
       <c r="AP58">
-        <v>8.0316511694180619E-3</v>
+        <v>7.6821403633477812E-3</v>
       </c>
       <c r="AQ58">
-        <v>4.1866663283612552E-3</v>
+        <v>2.2147959112184309E-2</v>
       </c>
       <c r="AR58">
-        <v>0.73238348824898791</v>
+        <v>0.6664021975993526</v>
       </c>
       <c r="AS58">
-        <v>30.512326457271001</v>
-      </c>
-      <c r="AT58" s="9">
+        <v>47.569670574336783</v>
+      </c>
+      <c r="AT58" s="2">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
+      <c r="AU58" s="1"/>
     </row>
     <row r="59" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>0.17877049458235161</v>
+        <v>6.0665085926573631E-2</v>
       </c>
       <c r="B59">
-        <v>0.6133644174327233</v>
+        <v>0.47272629839424268</v>
       </c>
       <c r="C59">
-        <v>0.19186906865394299</v>
+        <v>0.55233849554789594</v>
       </c>
       <c r="D59">
-        <v>2.8186713031514558E-3</v>
+        <v>3.2167713448302241E-3</v>
       </c>
       <c r="E59">
-        <v>2.1802113281694381E-2</v>
+        <v>6.7518868747691533E-3</v>
       </c>
       <c r="F59">
-        <v>0.29862934725895268</v>
+        <v>3.2038273930865217E-2</v>
       </c>
       <c r="G59">
-        <v>0.52083594338879247</v>
+        <v>0.7443096289250738</v>
       </c>
       <c r="H59">
-        <v>0.58741646709852691</v>
+        <v>3.3683522886886919E-2</v>
       </c>
       <c r="I59">
-        <v>0.39444712057872477</v>
+        <v>0.60436326203495694</v>
       </c>
       <c r="J59">
-        <v>8.3700918883575476E-2</v>
+        <v>4.6327698980049743E-2</v>
       </c>
       <c r="K59">
-        <v>6.085202390806646E-2</v>
+        <v>2.080651039608393E-2</v>
       </c>
       <c r="L59">
-        <v>2.1705301877836228E-3</v>
+        <v>3.2312745700035332E-2</v>
       </c>
       <c r="M59">
-        <v>1.814155694593156E-3</v>
+        <v>1.8887187521105318E-2</v>
       </c>
       <c r="N59">
-        <v>1.2775934700629059E-2</v>
+        <v>8.7909160222302673E-3</v>
       </c>
       <c r="O59">
-        <v>0.555279684176198</v>
+        <v>0.54553465354961694</v>
       </c>
       <c r="P59">
-        <v>0.18977823873648211</v>
+        <v>4.1010297960852843E-2</v>
       </c>
       <c r="Q59">
-        <v>1.2273604518983981E-3</v>
+        <v>4.8177347438859423E-2</v>
       </c>
       <c r="R59">
-        <v>2.5703759718509071E-2</v>
+        <v>3.2153765943582692E-2</v>
       </c>
       <c r="S59">
-        <v>1.212305287422967E-2</v>
+        <v>1.465291220286746E-3</v>
       </c>
       <c r="T59">
-        <v>2.2305997671923421E-2</v>
+        <v>1.6841919612880001E-2</v>
       </c>
       <c r="U59">
-        <v>0.44852038554530871</v>
+        <v>0.33200572852343918</v>
       </c>
       <c r="V59">
-        <v>0.16859608908675641</v>
+        <v>3.7069671081555761E-2</v>
       </c>
       <c r="W59">
-        <v>2.7956909580341131E-2</v>
+        <v>7.1133894923729374E-2</v>
       </c>
       <c r="X59">
-        <v>2.4513958111513942E-3</v>
+        <v>4.0451876817633589E-3</v>
       </c>
       <c r="Y59">
-        <v>9.3890470115705095E-3</v>
+        <v>1.3523711440632251E-3</v>
       </c>
       <c r="Z59">
-        <v>1.0569079394492169E-3</v>
+        <v>1.355887382815784E-2</v>
       </c>
       <c r="AA59">
-        <v>0.11248993779002479</v>
+        <v>3.2752540723000378E-2</v>
       </c>
       <c r="AB59">
-        <v>1.27995503204822E-2</v>
+        <v>7.8078638621362162E-2</v>
       </c>
       <c r="AC59">
-        <v>4.5382720162878983E-2</v>
+        <v>5.7632973504134273E-2</v>
       </c>
       <c r="AD59">
-        <v>6.5637424036708754E-3</v>
+        <v>5.7980528530883341E-3</v>
       </c>
       <c r="AE59">
-        <v>1.7947201810540579E-2</v>
+        <v>5.6674181546491342E-4</v>
       </c>
       <c r="AF59">
-        <v>0.31214559737667991</v>
+        <v>0.43839579580866328</v>
       </c>
       <c r="AG59">
-        <v>0.13793494192439679</v>
+        <v>7.8144553172492304E-2</v>
       </c>
       <c r="AH59">
-        <v>3.6577804546072449E-3</v>
+        <v>2.40672268807102E-2</v>
       </c>
       <c r="AI59">
-        <v>1.0494979762065079E-2</v>
+        <v>3.7801840931906049E-2</v>
       </c>
       <c r="AJ59">
-        <v>1.8290146349311271E-2</v>
+        <v>1.3676415548283411E-2</v>
       </c>
       <c r="AK59">
-        <v>2.1046084198721639E-2</v>
+        <v>3.5929406215859661E-3</v>
       </c>
       <c r="AL59">
-        <v>0.34985261397006318</v>
+        <v>9.0318204968601407E-2</v>
       </c>
       <c r="AM59">
-        <v>0.14239724557561409</v>
+        <v>6.902522065626171E-2</v>
       </c>
       <c r="AN59">
-        <v>7.0690883847908392E-2</v>
+        <v>1.237031947023043E-2</v>
       </c>
       <c r="AO59">
-        <v>7.4891355274441684E-2</v>
+        <v>9.774176640690949E-3</v>
       </c>
       <c r="AP59">
-        <v>1.415018132722427E-2</v>
+        <v>1.1623803599190781E-2</v>
       </c>
       <c r="AQ59">
-        <v>8.0473920143672999E-4</v>
+        <v>2.03861121172998E-2</v>
       </c>
       <c r="AR59">
-        <v>0.30370617476714901</v>
+        <v>0.96027356293895683</v>
       </c>
       <c r="AS59">
-        <v>44.301270957379693</v>
-      </c>
-      <c r="AT59" s="9">
+        <v>47.731715945093292</v>
+      </c>
+      <c r="AT59" s="2">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
+      <c r="AU59" s="1"/>
     </row>
     <row r="60" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="AT60" s="9">
+      <c r="A60">
+        <v>0.16219245526942669</v>
+      </c>
+      <c r="B60">
+        <v>0.12941459784162099</v>
+      </c>
+      <c r="C60">
+        <v>1.3343855281409359E-2</v>
+      </c>
+      <c r="D60">
+        <v>3.1629275531599131E-3</v>
+      </c>
+      <c r="E60">
+        <v>5.244943294882674E-3</v>
+      </c>
+      <c r="F60">
+        <v>0.70103564271928542</v>
+      </c>
+      <c r="G60">
+        <v>8.2541560688676463E-2</v>
+      </c>
+      <c r="H60">
+        <v>0.18603477814362859</v>
+      </c>
+      <c r="I60">
+        <v>0.74644441533891881</v>
+      </c>
+      <c r="J60">
+        <v>0.1681442150880475</v>
+      </c>
+      <c r="K60">
+        <v>7.9680780882232197E-2</v>
+      </c>
+      <c r="L60">
+        <v>6.5521578359597266E-2</v>
+      </c>
+      <c r="M60">
+        <v>1.7510693221554699E-2</v>
+      </c>
+      <c r="N60">
+        <v>6.4372324876934648E-3</v>
+      </c>
+      <c r="O60">
+        <v>0.66403841711380063</v>
+      </c>
+      <c r="P60">
+        <v>2.2560098234820442E-2</v>
+      </c>
+      <c r="Q60">
+        <v>2.7254523550371453E-4</v>
+      </c>
+      <c r="R60">
+        <v>1.9965140814615041E-2</v>
+      </c>
+      <c r="S60">
+        <v>3.1442071154139388E-4</v>
+      </c>
+      <c r="T60">
+        <v>1.828101837393686E-2</v>
+      </c>
+      <c r="U60">
+        <v>0.68816218013119745</v>
+      </c>
+      <c r="V60">
+        <v>0.14354382843533101</v>
+      </c>
+      <c r="W60">
+        <v>5.3556372887725121E-2</v>
+      </c>
+      <c r="X60">
+        <v>7.0321952047990688E-2</v>
+      </c>
+      <c r="Y60">
+        <v>1.342561567139069E-2</v>
+      </c>
+      <c r="Z60">
+        <v>2.3206569587973989E-2</v>
+      </c>
+      <c r="AA60">
+        <v>0.12078908181183021</v>
+      </c>
+      <c r="AB60">
+        <v>1.2986306919215731E-2</v>
+      </c>
+      <c r="AC60">
+        <v>5.8429065492033611E-2</v>
+      </c>
+      <c r="AD60">
+        <v>2.2182626656987409E-2</v>
+      </c>
+      <c r="AE60">
+        <v>1.352196059903348E-2</v>
+      </c>
+      <c r="AF60">
+        <v>0.26901900679638058</v>
+      </c>
+      <c r="AG60">
+        <v>0.1044713079838686</v>
+      </c>
+      <c r="AH60">
+        <v>5.3261442019813442E-2</v>
+      </c>
+      <c r="AI60">
+        <v>4.7401938990117971E-2</v>
+      </c>
+      <c r="AJ60">
+        <v>1.265966685698915E-2</v>
+      </c>
+      <c r="AK60">
+        <v>5.5946829778609989E-3</v>
+      </c>
+      <c r="AL60">
+        <v>0.25295898572824582</v>
+      </c>
+      <c r="AM60">
+        <v>0.12906165303595071</v>
+      </c>
+      <c r="AN60">
+        <v>1.0519419980512611E-2</v>
+      </c>
+      <c r="AO60">
+        <v>6.1292273475295901E-2</v>
+      </c>
+      <c r="AP60">
+        <v>2.4267638488172762E-3</v>
+      </c>
+      <c r="AQ60">
+        <v>3.4664326996320378E-3</v>
+      </c>
+      <c r="AR60">
+        <v>0.7504843615751553</v>
+      </c>
+      <c r="AS60">
+        <v>51.681438005353641</v>
+      </c>
+      <c r="AT60" s="2">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="AT61" s="9">
+      <c r="A61">
+        <v>0.1914388246771897</v>
+      </c>
+      <c r="B61">
+        <v>0.22435116628800389</v>
+      </c>
+      <c r="C61">
+        <v>0.11738458753879399</v>
+      </c>
+      <c r="D61">
+        <v>3.73586988904093E-3</v>
+      </c>
+      <c r="E61">
+        <v>1.6733771124780701E-2</v>
+      </c>
+      <c r="F61">
+        <v>0.28741053951415602</v>
+      </c>
+      <c r="G61">
+        <v>0.81400275172747216</v>
+      </c>
+      <c r="H61">
+        <v>9.839923079102797E-2</v>
+      </c>
+      <c r="I61">
+        <v>0.53236865734067351</v>
+      </c>
+      <c r="J61">
+        <v>5.714615535475609E-2</v>
+      </c>
+      <c r="K61">
+        <v>6.5398683675479755E-2</v>
+      </c>
+      <c r="L61">
+        <v>2.7685583369284322E-2</v>
+      </c>
+      <c r="M61">
+        <v>1.454719049235287E-2</v>
+      </c>
+      <c r="N61">
+        <v>8.3680251222636726E-3</v>
+      </c>
+      <c r="O61">
+        <v>0.35094822375262402</v>
+      </c>
+      <c r="P61">
+        <v>0.12055295045310919</v>
+      </c>
+      <c r="Q61">
+        <v>3.928170719033628E-2</v>
+      </c>
+      <c r="R61">
+        <v>5.555639655385107E-2</v>
+      </c>
+      <c r="S61">
+        <v>1.9923431376489109E-2</v>
+      </c>
+      <c r="T61">
+        <v>3.3262356653058879E-3</v>
+      </c>
+      <c r="U61">
+        <v>0.33916716881634118</v>
+      </c>
+      <c r="V61">
+        <v>3.9330910223077033E-2</v>
+      </c>
+      <c r="W61">
+        <v>1.323721386744661E-2</v>
+      </c>
+      <c r="X61">
+        <v>4.2084234973269741E-2</v>
+      </c>
+      <c r="Y61">
+        <v>4.0830130777507303E-3</v>
+      </c>
+      <c r="Z61">
+        <v>1.6026495735154848E-2</v>
+      </c>
+      <c r="AA61">
+        <v>9.3728641994805739E-2</v>
+      </c>
+      <c r="AB61">
+        <v>2.6680220943044682E-2</v>
+      </c>
+      <c r="AC61">
+        <v>5.8619629641051907E-3</v>
+      </c>
+      <c r="AD61">
+        <v>4.8924458819659851E-3</v>
+      </c>
+      <c r="AE61">
+        <v>2.0912638746523909E-2</v>
+      </c>
+      <c r="AF61">
+        <v>0.36110111510639942</v>
+      </c>
+      <c r="AG61">
+        <v>0.17501318205113769</v>
+      </c>
+      <c r="AH61">
+        <v>1.848968091391541E-2</v>
+      </c>
+      <c r="AI61">
+        <v>6.8320533319862722E-2</v>
+      </c>
+      <c r="AJ61">
+        <v>6.2843147038141034E-3</v>
+      </c>
+      <c r="AK61">
+        <v>1.458314299701617E-2</v>
+      </c>
+      <c r="AL61">
+        <v>0.61712464326788252</v>
+      </c>
+      <c r="AM61">
+        <v>0.24125637940254591</v>
+      </c>
+      <c r="AN61">
+        <v>7.3445717072590164E-2</v>
+      </c>
+      <c r="AO61">
+        <v>5.0082179288248957E-2</v>
+      </c>
+      <c r="AP61">
+        <v>2.3524952919933371E-2</v>
+      </c>
+      <c r="AQ61">
+        <v>8.2167020586413342E-3</v>
+      </c>
+      <c r="AR61">
+        <v>0.55339204670120112</v>
+      </c>
+      <c r="AS61">
+        <v>50.538413264484547</v>
+      </c>
+      <c r="AT61" s="2">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="AT62" s="9">
+      <c r="AT62" s="2">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="AT63" s="9">
+      <c r="AT63" s="2">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="AT64" s="9">
+      <c r="AT64" s="2">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
     </row>
     <row r="65" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT65" s="9">
+      <c r="AT65" s="2">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
     <row r="66" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT66" s="9">
+      <c r="AT66" s="2">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
     </row>
     <row r="67" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT67" s="9">
+      <c r="AT67" s="2">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
     </row>
     <row r="68" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT68" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT68" s="2">
+        <f t="shared" ref="AT68:AT99" si="1">AT67+1</f>
         <v>67</v>
       </c>
     </row>
     <row r="69" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT69" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT69" s="2">
+        <f t="shared" si="1"/>
         <v>68</v>
       </c>
     </row>
     <row r="70" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT70" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT70" s="2">
+        <f t="shared" si="1"/>
         <v>69</v>
       </c>
     </row>
     <row r="71" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT71" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT71" s="2">
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
     </row>
     <row r="72" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT72" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT72" s="2">
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
     </row>
     <row r="73" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT73" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT73" s="2">
+        <f t="shared" si="1"/>
         <v>72</v>
       </c>
     </row>
     <row r="74" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT74" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT74" s="2">
+        <f t="shared" si="1"/>
         <v>73</v>
       </c>
     </row>
     <row r="75" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT75" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT75" s="2">
+        <f t="shared" si="1"/>
         <v>74</v>
       </c>
     </row>
     <row r="76" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT76" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT76" s="2">
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
     </row>
     <row r="77" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT77" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT77" s="2">
+        <f t="shared" si="1"/>
         <v>76</v>
       </c>
     </row>
     <row r="78" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT78" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT78" s="2">
+        <f t="shared" si="1"/>
         <v>77</v>
       </c>
     </row>
     <row r="79" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT79" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT79" s="2">
+        <f t="shared" si="1"/>
         <v>78</v>
       </c>
     </row>
     <row r="80" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT80" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT80" s="2">
+        <f t="shared" si="1"/>
         <v>79</v>
       </c>
     </row>
     <row r="81" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT81" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT81" s="2">
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
     <row r="82" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT82" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT82" s="2">
+        <f t="shared" si="1"/>
         <v>81</v>
       </c>
     </row>
     <row r="83" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT83" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT83" s="2">
+        <f t="shared" si="1"/>
         <v>82</v>
       </c>
     </row>
     <row r="84" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT84" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT84" s="2">
+        <f t="shared" si="1"/>
         <v>83</v>
       </c>
     </row>
     <row r="85" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT85" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT85" s="2">
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
     </row>
     <row r="86" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT86" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT86" s="2">
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
     </row>
     <row r="87" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT87" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT87" s="2">
+        <f t="shared" si="1"/>
         <v>86</v>
       </c>
     </row>
     <row r="88" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT88" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT88" s="2">
+        <f t="shared" si="1"/>
         <v>87</v>
       </c>
     </row>
     <row r="89" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT89" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT89" s="2">
+        <f t="shared" si="1"/>
         <v>88</v>
       </c>
     </row>
     <row r="90" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT90" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT90" s="2">
+        <f t="shared" si="1"/>
         <v>89</v>
       </c>
     </row>
     <row r="91" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT91" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT91" s="2">
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
     </row>
     <row r="92" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT92" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT92" s="2">
+        <f t="shared" si="1"/>
         <v>91</v>
       </c>
     </row>
     <row r="93" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT93" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT93" s="2">
+        <f t="shared" si="1"/>
         <v>92</v>
       </c>
     </row>
     <row r="94" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT94" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT94" s="2">
+        <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
     <row r="95" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT95" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT95" s="2">
+        <f t="shared" si="1"/>
         <v>94</v>
       </c>
     </row>
     <row r="96" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT96" s="9">
-        <f t="shared" si="0"/>
+      <c r="AT96" s="2">
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="AT97" s="9">
-        <f t="shared" si="0"/>
+    <row r="97" spans="46:46" x14ac:dyDescent="0.2">
+      <c r="AT97" s="2">
+        <f t="shared" si="1"/>
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="AT98" s="9">
-        <f t="shared" si="0"/>
+    <row r="98" spans="46:46" x14ac:dyDescent="0.2">
+      <c r="AT98" s="2">
+        <f t="shared" si="1"/>
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="AT99" s="9">
-        <f t="shared" si="0"/>
+    <row r="99" spans="46:46" x14ac:dyDescent="0.2">
+      <c r="AT99" s="2">
+        <f t="shared" si="1"/>
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="AT100" s="9">
-        <f t="shared" si="0"/>
+    <row r="100" spans="46:46" x14ac:dyDescent="0.2">
+      <c r="AT100" s="2">
+        <f>AT99+1</f>
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="AT101" s="9">
-        <f t="shared" si="0"/>
+    <row r="101" spans="46:46" x14ac:dyDescent="0.2">
+      <c r="AT101" s="2">
+        <f t="shared" ref="AT101" si="2">AT100+1</f>
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="102" spans="46:46" x14ac:dyDescent="0.2">
       <c r="AT102" s="9"/>
     </row>
-    <row r="103" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="103" spans="46:46" x14ac:dyDescent="0.2">
       <c r="AT103" s="9"/>
     </row>
-    <row r="104" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="104" spans="46:46" x14ac:dyDescent="0.2">
       <c r="AT104" s="9"/>
     </row>
-    <row r="105" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="105" spans="46:46" x14ac:dyDescent="0.2">
       <c r="AT105" s="9"/>
     </row>
-    <row r="106" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="AT106" s="9"/>
-    </row>
-    <row r="107" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A107">
-        <f>MIN(A2:A105)</f>
-        <v>9.1200749286037832E-4</v>
-      </c>
-      <c r="B107">
-        <f>MIN(B2:B105)</f>
-        <v>2.6703744601114239E-3</v>
-      </c>
-      <c r="C107">
-        <f>MIN(C2:C105)</f>
-        <v>1.5042004789833641E-3</v>
-      </c>
-      <c r="D107">
-        <f>MIN(D2:D105)</f>
-        <v>1.7683564719291401E-3</v>
-      </c>
-      <c r="E107">
-        <f>MIN(E2:E105)</f>
-        <v>2.4639355020977601E-3</v>
-      </c>
-      <c r="F107">
-        <f>MIN(F2:F105)</f>
-        <v>4.9577222606913551E-3</v>
-      </c>
-      <c r="G107">
-        <f>MIN(G2:G105)</f>
-        <v>2.077092723834539E-2</v>
-      </c>
-      <c r="H107">
-        <f>MIN(H2:H105)</f>
-        <v>8.3916481920353059E-3</v>
-      </c>
-      <c r="I107">
-        <f>MIN(I2:I105)</f>
-        <v>2.342912760689986E-4</v>
-      </c>
-      <c r="J107">
-        <f>MIN(J2:J105)</f>
-        <v>1.2748407690540971E-3</v>
-      </c>
-      <c r="K107">
-        <f>MIN(K2:K105)</f>
-        <v>4.3263207289065816E-3</v>
-      </c>
-      <c r="L107">
-        <f>MIN(L2:L105)</f>
-        <v>2.25772499597332E-5</v>
-      </c>
-      <c r="M107">
-        <f>MIN(M2:M105)</f>
-        <v>2.5628749472644818E-4</v>
-      </c>
-      <c r="N107">
-        <f>MIN(N2:N105)</f>
-        <v>4.0112697286892319E-4</v>
-      </c>
-      <c r="O107">
-        <f>MIN(O2:O105)</f>
-        <v>0.30705090310753552</v>
-      </c>
-      <c r="P107">
-        <f>MIN(P2:P105)</f>
-        <v>3.4788724925084169E-3</v>
-      </c>
-      <c r="Q107">
-        <f>MIN(Q2:Q105)</f>
-        <v>2.7254523550371453E-4</v>
-      </c>
-      <c r="R107">
-        <f>MIN(R2:R105)</f>
-        <v>1.0001842472339259E-3</v>
-      </c>
-      <c r="S107">
-        <f>MIN(S2:S105)</f>
-        <v>1.7053918216936311E-4</v>
-      </c>
-      <c r="T107">
-        <f>MIN(T2:T105)</f>
-        <v>4.3184525235314688E-4</v>
-      </c>
-      <c r="U107">
-        <f>MIN(U2:U105)</f>
-        <v>0.31763340591126471</v>
-      </c>
-      <c r="V107">
-        <f>MIN(V2:V105)</f>
-        <v>1.3668569326076849E-3</v>
-      </c>
-      <c r="W107">
-        <f>MIN(W2:W105)</f>
-        <v>2.3957253291987719E-4</v>
-      </c>
-      <c r="X107">
-        <f>MIN(X2:X105)</f>
-        <v>1.747984293506435E-3</v>
-      </c>
-      <c r="Y107">
-        <f>MIN(Y2:Y105)</f>
-        <v>1.9754839422765069E-4</v>
-      </c>
-      <c r="Z107">
-        <f>MIN(Z2:Z105)</f>
-        <v>9.4615811454937249E-5</v>
-      </c>
-      <c r="AA107">
-        <f>MIN(AA2:AA105)</f>
-        <v>9.3714576814957103E-3</v>
-      </c>
-      <c r="AB107">
-        <f>MIN(AB2:AB105)</f>
-        <v>2.1323551616689201E-4</v>
-      </c>
-      <c r="AC107">
-        <f>MIN(AC2:AC105)</f>
-        <v>1.1155761600258019E-3</v>
-      </c>
-      <c r="AD107">
-        <f>MIN(AD2:AD105)</f>
-        <v>9.2326954102878175E-5</v>
-      </c>
-      <c r="AE107">
-        <f>MIN(AE2:AE105)</f>
-        <v>3.2522671664910737E-4</v>
-      </c>
-      <c r="AF107">
-        <f>MIN(AF2:AF105)</f>
-        <v>1.4816318222834021E-2</v>
-      </c>
-      <c r="AG107">
-        <f>MIN(AG2:AG105)</f>
-        <v>7.6834455476513797E-3</v>
-      </c>
-      <c r="AH107">
-        <f>MIN(AH2:AH105)</f>
-        <v>9.8282938630765097E-4</v>
-      </c>
-      <c r="AI107">
-        <f>MIN(AI2:AI105)</f>
-        <v>7.1608950590809335E-4</v>
-      </c>
-      <c r="AJ107">
-        <f>MIN(AJ2:AJ105)</f>
-        <v>2.7932755382555031E-4</v>
-      </c>
-      <c r="AK107">
-        <f>MIN(AK2:AK105)</f>
-        <v>3.6527914369414988E-4</v>
-      </c>
-      <c r="AL107">
-        <f>MIN(AL2:AL105)</f>
-        <v>3.581729121851665E-2</v>
-      </c>
-      <c r="AM107">
-        <f>MIN(AM2:AM105)</f>
-        <v>6.4914776702367106E-3</v>
-      </c>
-      <c r="AN107">
-        <f>MIN(AN2:AN105)</f>
-        <v>9.5104817921684126E-4</v>
-      </c>
-      <c r="AO107">
-        <f>MIN(AO2:AO105)</f>
-        <v>1.213889686106973E-4</v>
-      </c>
-      <c r="AP107">
-        <f>MIN(AP2:AP105)</f>
-        <v>4.2764994812932451E-4</v>
-      </c>
-      <c r="AQ107">
-        <f>MIN(AQ2:AQ105)</f>
-        <v>3.2698309688753698E-4</v>
-      </c>
-      <c r="AR107">
-        <f>MIN(AR2:AR105)</f>
-        <v>4.4796870203235417E-2</v>
-      </c>
-      <c r="AS107">
-        <f>MIN(AS2:AS105)</f>
-        <v>1.1074691591477459</v>
-      </c>
-    </row>
-    <row r="108" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A108">
-        <f>MAX(A4:A107)</f>
-        <v>0.19578481000823919</v>
-      </c>
-      <c r="B108">
-        <f>MAX(B4:B107)</f>
-        <v>0.98182080582845999</v>
-      </c>
-      <c r="C108">
-        <f>MAX(C4:C107)</f>
-        <v>0.99372299235417905</v>
-      </c>
-      <c r="D108">
-        <f>MAX(D4:D107)</f>
-        <v>8.2482710628555746E-3</v>
-      </c>
-      <c r="E108">
-        <f>MAX(E4:E107)</f>
-        <v>2.7206158463695181E-2</v>
-      </c>
-      <c r="F108">
-        <f>MAX(F4:F107)</f>
-        <v>0.98785655441021336</v>
-      </c>
-      <c r="G108">
-        <f>MAX(G4:G107)</f>
-        <v>0.97012328240860157</v>
-      </c>
-      <c r="H108">
-        <f>MAX(H4:H107)</f>
-        <v>0.99944097759397688</v>
-      </c>
-      <c r="I108">
-        <f>MAX(I4:I107)</f>
-        <v>0.74644441533891881</v>
-      </c>
-      <c r="J108">
-        <f>MAX(J4:J107)</f>
-        <v>0.97668883515212834</v>
-      </c>
-      <c r="K108">
-        <f>MAX(K4:K107)</f>
-        <v>0.27602084930352749</v>
-      </c>
-      <c r="L108">
-        <f>MAX(L4:L107)</f>
-        <v>0.25877878874422799</v>
-      </c>
-      <c r="M108">
-        <f>MAX(M4:M107)</f>
-        <v>9.9694582695835615E-2</v>
-      </c>
-      <c r="N108">
-        <f>MAX(N4:N107)</f>
-        <v>8.3996347521141657E-2</v>
-      </c>
-      <c r="O108">
-        <f>MAX(O4:O107)</f>
-        <v>0.71288308714835247</v>
-      </c>
-      <c r="P108">
-        <f>MAX(P4:P107)</f>
-        <v>0.81938119069666848</v>
-      </c>
-      <c r="Q108">
-        <f>MAX(Q4:Q107)</f>
-        <v>0.30775060747468269</v>
-      </c>
-      <c r="R108">
-        <f>MAX(R4:R107)</f>
-        <v>0.29268559871659128</v>
-      </c>
-      <c r="S108">
-        <f>MAX(S4:S107)</f>
-        <v>9.5156480272306998E-2</v>
-      </c>
-      <c r="T108">
-        <f>MAX(T4:T107)</f>
-        <v>9.7067777803672331E-2</v>
-      </c>
-      <c r="U108">
-        <f>MAX(U4:U107)</f>
-        <v>0.741883365822117</v>
-      </c>
-      <c r="V108">
-        <f>MAX(V4:V107)</f>
-        <v>0.97745175030552789</v>
-      </c>
-      <c r="W108">
-        <f>MAX(W4:W107)</f>
-        <v>0.30320119619793828</v>
-      </c>
-      <c r="X108">
-        <f>MAX(X4:X107)</f>
-        <v>0.31798840970224429</v>
-      </c>
-      <c r="Y108">
-        <f>MAX(Y4:Y107)</f>
-        <v>9.1730785413313046E-2</v>
-      </c>
-      <c r="Z108">
-        <f>MAX(Z4:Z107)</f>
-        <v>9.1713768408342958E-2</v>
-      </c>
-      <c r="AA108">
-        <f>MAX(AA4:AA107)</f>
-        <v>0.9338262935284265</v>
-      </c>
-      <c r="AB108">
-        <f>MAX(AB4:AB107)</f>
-        <v>0.32196086832130782</v>
-      </c>
-      <c r="AC108">
-        <f>MAX(AC4:AC107)</f>
-        <v>0.27769881368615978</v>
-      </c>
-      <c r="AD108">
-        <f>MAX(AD4:AD107)</f>
-        <v>8.6355553327244136E-2</v>
-      </c>
-      <c r="AE108">
-        <f>MAX(AE4:AE107)</f>
-        <v>9.1080614217186176E-2</v>
-      </c>
-      <c r="AF108">
-        <f>MAX(AF4:AF107)</f>
-        <v>0.4953457882037266</v>
-      </c>
-      <c r="AG108">
-        <f>MAX(AG4:AG107)</f>
-        <v>0.95001736384242319</v>
-      </c>
-      <c r="AH108">
-        <f>MAX(AH4:AH107)</f>
-        <v>0.3247507161258546</v>
-      </c>
-      <c r="AI108">
-        <f>MAX(AI4:AI107)</f>
-        <v>0.30313399769979688</v>
-      </c>
-      <c r="AJ108">
-        <f>MAX(AJ4:AJ107)</f>
-        <v>9.8454095587671014E-2</v>
-      </c>
-      <c r="AK108">
-        <f>MAX(AK4:AK107)</f>
-        <v>8.8823551670109649E-2</v>
-      </c>
-      <c r="AL108">
-        <f>MAX(AL4:AL107)</f>
-        <v>0.74424878381239645</v>
-      </c>
-      <c r="AM108">
-        <f>MAX(AM4:AM107)</f>
-        <v>0.97076237527343701</v>
-      </c>
-      <c r="AN108">
-        <f>MAX(AN4:AN107)</f>
-        <v>0.3112860980456742</v>
-      </c>
-      <c r="AO108">
-        <f>MAX(AO4:AO107)</f>
-        <v>0.32181015720016198</v>
-      </c>
-      <c r="AP108">
-        <f>MAX(AP4:AP107)</f>
-        <v>9.769252671524993E-2</v>
-      </c>
-      <c r="AQ108">
-        <f>MAX(AQ4:AQ107)</f>
-        <v>8.9790503510623385E-2</v>
-      </c>
-      <c r="AR108">
-        <f>MAX(AR4:AR107)</f>
-        <v>0.97121562751642831</v>
-      </c>
-      <c r="AS108">
-        <f>MAX(AS4:AS107)</f>
-        <v>51.681438005353641</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AU108">
-    <sortCondition ref="AS2:AS108"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AU107">
+    <sortCondition ref="AS2:AS107"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9737,7 +9641,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9939,7 +9843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8853FD4-E1D4-0347-8106-6FB88BEFF854}">
   <dimension ref="A1:AV43"/>
   <sheetViews>
-    <sheetView topLeftCell="AM19" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="AU43" sqref="AU43"/>
     </sheetView>
   </sheetViews>

</xml_diff>